<commit_message>
Update for Jinx 0.1.1 release
</commit_message>
<xml_diff>
--- a/examples/swap-pricer.xlsx
+++ b/examples/swap-pricer.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\strata-excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\strata-excel\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="3953"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="3953" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Market Data" sheetId="2" r:id="rId1"/>
@@ -750,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -769,7 +769,7 @@
     <row r="2" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="str">
         <f>_xll.og.CurveCalibrator.calibrate(_xll.og.CurveCalibrator.standard(),B8,C4,C6)</f>
-        <v>ImmutableRatesProvider@9</v>
+        <v>ImmutableRatesProvider@3</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.45">
@@ -786,7 +786,7 @@
       </c>
       <c r="C4" s="17" t="str">
         <f>_xll.og.MarketData.combinedWith(C5,D5)</f>
-        <v>ImmutableMarketData@22</v>
+        <v>ImmutableMarketData@7</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -795,11 +795,11 @@
       </c>
       <c r="C5" s="12" t="str">
         <f>_xll.og.MarketData.of(C3,E14:E27,D14:D27)</f>
-        <v>ImmutableMarketData@21</v>
+        <v>ImmutableMarketData@6</v>
       </c>
       <c r="D5" s="12" t="str">
         <f>_xll.og.MarketData.of(C3,K14:K23,J14:J23)</f>
-        <v>ImmutableMarketData@20</v>
+        <v>ImmutableMarketData@1</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.45">
@@ -808,13 +808,13 @@
       </c>
       <c r="C6" s="12" t="str">
         <f>_xll.og.ReferenceData.standard()</f>
-        <v>ImmutableReferenceData@10</v>
+        <v>ImmutableReferenceData@1</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B8" s="16" t="str">
         <f>_xll.og.CurveGroupDefinition.of(C9,C10:D10,C11:D11)</f>
-        <v>CurveGroupDefinition@12</v>
+        <v>CurveGroupDefinition@1</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.45">
@@ -831,11 +831,11 @@
       </c>
       <c r="C10" s="12" t="str">
         <f>B38</f>
-        <v>CurveGroupEntry@16</v>
+        <v>CurveGroupEntry@2</v>
       </c>
       <c r="D10" s="12" t="str">
         <f>H38</f>
-        <v>CurveGroupEntry@15</v>
+        <v>CurveGroupEntry@1</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.45">
@@ -844,11 +844,11 @@
       </c>
       <c r="C11" s="12" t="str">
         <f>B29</f>
-        <v>InterpolatedNodalCurveDefinition@16</v>
+        <v>InterpolatedNodalCurveDefinition@2</v>
       </c>
       <c r="D11" s="12" t="str">
         <f>H29</f>
-        <v>InterpolatedNodalCurveDefinition@15</v>
+        <v>InterpolatedNodalCurveDefinition@1</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.45">
@@ -895,11 +895,11 @@
       </c>
       <c r="E14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B14&amp;"."&amp;C14)</f>
-        <v>QuoteId@153</v>
+        <v>QuoteId@22</v>
       </c>
       <c r="F14" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C14,B14),E14)</f>
-        <v>FixedOvernightSwapCurveNode@84</v>
+        <v>FixedOvernightSwapCurveNode@14</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>75</v>
@@ -912,11 +912,11 @@
       </c>
       <c r="K14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H14&amp;"."&amp;I14)</f>
-        <v>QuoteId@135</v>
+        <v>QuoteId@10</v>
       </c>
       <c r="L14" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I14,H14),K14)</f>
-        <v>FixedIborSwapCurveNode@71</v>
+        <v>FixedIborSwapCurveNode@10</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.45">
@@ -931,11 +931,11 @@
       </c>
       <c r="E15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B15&amp;"."&amp;C15)</f>
-        <v>QuoteId@142</v>
+        <v>QuoteId@12</v>
       </c>
       <c r="F15" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C15,B15),E15)</f>
-        <v>FixedOvernightSwapCurveNode@71</v>
+        <v>FixedOvernightSwapCurveNode@4</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>75</v>
@@ -948,11 +948,11 @@
       </c>
       <c r="K15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H15&amp;"."&amp;I15)</f>
-        <v>QuoteId@140</v>
+        <v>QuoteId@9</v>
       </c>
       <c r="L15" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I15,H15),K15)</f>
-        <v>FixedIborSwapCurveNode@70</v>
+        <v>FixedIborSwapCurveNode@9</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.45">
@@ -967,11 +967,11 @@
       </c>
       <c r="E16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B16&amp;"."&amp;C16)</f>
-        <v>QuoteId@144</v>
+        <v>QuoteId@11</v>
       </c>
       <c r="F16" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C16,B16),E16)</f>
-        <v>FixedOvernightSwapCurveNode@72</v>
+        <v>FixedOvernightSwapCurveNode@1</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>75</v>
@@ -984,11 +984,11 @@
       </c>
       <c r="K16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H16&amp;"."&amp;I16)</f>
-        <v>QuoteId@136</v>
+        <v>QuoteId@5</v>
       </c>
       <c r="L16" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I16,H16),K16)</f>
-        <v>FixedIborSwapCurveNode@66</v>
+        <v>FixedIborSwapCurveNode@7</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.45">
@@ -1003,11 +1003,11 @@
       </c>
       <c r="E17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B17&amp;"."&amp;C17)</f>
-        <v>QuoteId@141</v>
+        <v>QuoteId@13</v>
       </c>
       <c r="F17" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C17,B17),E17)</f>
-        <v>FixedOvernightSwapCurveNode@74</v>
+        <v>FixedOvernightSwapCurveNode@2</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>75</v>
@@ -1020,11 +1020,11 @@
       </c>
       <c r="K17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H17&amp;"."&amp;I17)</f>
-        <v>QuoteId@134</v>
+        <v>QuoteId@6</v>
       </c>
       <c r="L17" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I17,H17),K17)</f>
-        <v>FixedIborSwapCurveNode@65</v>
+        <v>FixedIborSwapCurveNode@5</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.45">
@@ -1039,11 +1039,11 @@
       </c>
       <c r="E18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B18&amp;"."&amp;C18)</f>
-        <v>QuoteId@143</v>
+        <v>QuoteId@14</v>
       </c>
       <c r="F18" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C18,B18),E18)</f>
-        <v>FixedOvernightSwapCurveNode@73</v>
+        <v>FixedOvernightSwapCurveNode@3</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>75</v>
@@ -1056,11 +1056,11 @@
       </c>
       <c r="K18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H18&amp;"."&amp;I18)</f>
-        <v>QuoteId@133</v>
+        <v>QuoteId@8</v>
       </c>
       <c r="L18" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I18,H18),K18)</f>
-        <v>FixedIborSwapCurveNode@64</v>
+        <v>FixedIborSwapCurveNode@8</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.45">
@@ -1075,11 +1075,11 @@
       </c>
       <c r="E19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B19&amp;"."&amp;C19)</f>
-        <v>QuoteId@145</v>
+        <v>QuoteId@15</v>
       </c>
       <c r="F19" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C19,B19),E19)</f>
-        <v>FixedOvernightSwapCurveNode@75</v>
+        <v>FixedOvernightSwapCurveNode@6</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>75</v>
@@ -1092,11 +1092,11 @@
       </c>
       <c r="K19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H19&amp;"."&amp;I19)</f>
-        <v>QuoteId@139</v>
+        <v>QuoteId@7</v>
       </c>
       <c r="L19" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I19,H19),K19)</f>
-        <v>FixedIborSwapCurveNode@69</v>
+        <v>FixedIborSwapCurveNode@6</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.45">
@@ -1111,11 +1111,11 @@
       </c>
       <c r="E20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B20&amp;"."&amp;C20)</f>
-        <v>QuoteId@147</v>
+        <v>QuoteId@16</v>
       </c>
       <c r="F20" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C20,B20),E20)</f>
-        <v>FixedOvernightSwapCurveNode@76</v>
+        <v>FixedOvernightSwapCurveNode@5</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>75</v>
@@ -1128,11 +1128,11 @@
       </c>
       <c r="K20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H20&amp;"."&amp;I20)</f>
-        <v>QuoteId@137</v>
+        <v>QuoteId@3</v>
       </c>
       <c r="L20" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I20,H20),K20)</f>
-        <v>FixedIborSwapCurveNode@67</v>
+        <v>FixedIborSwapCurveNode@3</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.45">
@@ -1147,11 +1147,11 @@
       </c>
       <c r="E21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B21&amp;"."&amp;C21)</f>
-        <v>QuoteId@146</v>
+        <v>QuoteId@20</v>
       </c>
       <c r="F21" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C21,B21),E21)</f>
-        <v>FixedOvernightSwapCurveNode@77</v>
+        <v>FixedOvernightSwapCurveNode@13</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>75</v>
@@ -1164,11 +1164,11 @@
       </c>
       <c r="K21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H21&amp;"."&amp;I21)</f>
-        <v>QuoteId@132</v>
+        <v>QuoteId@2</v>
       </c>
       <c r="L21" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I21,H21),K21)</f>
-        <v>FixedIborSwapCurveNode@63</v>
+        <v>FixedIborSwapCurveNode@4</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.45">
@@ -1183,11 +1183,11 @@
       </c>
       <c r="E22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B22&amp;"."&amp;C22)</f>
-        <v>QuoteId@148</v>
+        <v>QuoteId@17</v>
       </c>
       <c r="F22" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C22,B22),E22)</f>
-        <v>FixedOvernightSwapCurveNode@78</v>
+        <v>FixedOvernightSwapCurveNode@7</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>75</v>
@@ -1200,11 +1200,11 @@
       </c>
       <c r="K22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H22&amp;"."&amp;I22)</f>
-        <v>QuoteId@131</v>
+        <v>QuoteId@4</v>
       </c>
       <c r="L22" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I22,H22),K22)</f>
-        <v>FixedIborSwapCurveNode@62</v>
+        <v>FixedIborSwapCurveNode@1</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.45">
@@ -1219,11 +1219,11 @@
       </c>
       <c r="E23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B23&amp;"."&amp;C23)</f>
-        <v>QuoteId@149</v>
+        <v>QuoteId@18</v>
       </c>
       <c r="F23" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C23,B23),E23)</f>
-        <v>FixedOvernightSwapCurveNode@80</v>
+        <v>FixedOvernightSwapCurveNode@12</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>75</v>
@@ -1236,11 +1236,11 @@
       </c>
       <c r="K23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H23&amp;"."&amp;I23)</f>
-        <v>QuoteId@138</v>
+        <v>QuoteId@1</v>
       </c>
       <c r="L23" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I23,H23),K23)</f>
-        <v>FixedIborSwapCurveNode@68</v>
+        <v>FixedIborSwapCurveNode@2</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.45">
@@ -1255,11 +1255,11 @@
       </c>
       <c r="E24" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B24&amp;"."&amp;C24)</f>
-        <v>QuoteId@150</v>
+        <v>QuoteId@19</v>
       </c>
       <c r="F24" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C24,B24),E24)</f>
-        <v>FixedOvernightSwapCurveNode@79</v>
+        <v>FixedOvernightSwapCurveNode@9</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.45">
@@ -1274,11 +1274,11 @@
       </c>
       <c r="E25" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B25&amp;"."&amp;C25)</f>
-        <v>QuoteId@151</v>
+        <v>QuoteId@24</v>
       </c>
       <c r="F25" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C25,B25),E25)</f>
-        <v>FixedOvernightSwapCurveNode@81</v>
+        <v>FixedOvernightSwapCurveNode@11</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.45">
@@ -1293,11 +1293,11 @@
       </c>
       <c r="E26" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B26&amp;"."&amp;C26)</f>
-        <v>QuoteId@152</v>
+        <v>QuoteId@21</v>
       </c>
       <c r="F26" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C26,B26),E26)</f>
-        <v>FixedOvernightSwapCurveNode@82</v>
+        <v>FixedOvernightSwapCurveNode@8</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.45">
@@ -1312,21 +1312,21 @@
       </c>
       <c r="E27" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B27&amp;"."&amp;C27)</f>
-        <v>QuoteId@154</v>
+        <v>QuoteId@23</v>
       </c>
       <c r="F27" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C27,B27),E27)</f>
-        <v>FixedOvernightSwapCurveNode@83</v>
+        <v>FixedOvernightSwapCurveNode@10</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B29" s="16" t="str">
         <f>_xll.og.InterpolatedNodalCurveDefinition.build(B30:B36,C30:C36,F14:F27)</f>
-        <v>InterpolatedNodalCurveDefinition@16</v>
+        <v>InterpolatedNodalCurveDefinition@2</v>
       </c>
       <c r="H29" s="16" t="str">
         <f>_xll.og.InterpolatedNodalCurveDefinition.build(H30:H36,I30:I36,L14:L23)</f>
-        <v>InterpolatedNodalCurveDefinition@15</v>
+        <v>InterpolatedNodalCurveDefinition@1</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.45">
@@ -1430,11 +1430,11 @@
     <row r="38" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B38" s="16" t="str">
         <f>_xll.og.CurveGroupEntry.of(C39,C40,C41)</f>
-        <v>CurveGroupEntry@16</v>
+        <v>CurveGroupEntry@2</v>
       </c>
       <c r="H38" s="16" t="str">
         <f>_xll.og.CurveGroupEntry.of(I39,I40,I41)</f>
-        <v>CurveGroupEntry@15</v>
+        <v>CurveGroupEntry@1</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.45">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="C41" s="12" t="str">
         <f>_xll.og.OvernightIndex.of(D41)</f>
-        <v>ImmutableOvernightIndex@7</v>
+        <v>ImmutableOvernightIndex@1</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>62</v>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="I41" s="12" t="str">
         <f>_xll.og.IborIndex.of(J41)</f>
-        <v>ImmutableIborIndex@8</v>
+        <v>ImmutableIborIndex@1</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>71</v>
@@ -1496,7 +1496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1517,14 +1517,14 @@
       </c>
       <c r="C2" s="8" t="str">
         <f>_xll.og.ReferenceData.standard()</f>
-        <v>ImmutableReferenceData@9</v>
+        <v>ImmutableReferenceData@2</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>69</v>
       </c>
       <c r="F2" s="20" t="str">
         <f>_xll.og.DiscountingSwapProductPricer.DEFAULT()</f>
-        <v>DiscountingSwapProductPricer@4</v>
+        <v>DiscountingSwapProductPricer@1</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.45">
@@ -1533,14 +1533,14 @@
       </c>
       <c r="C3" s="8" t="str">
         <f>_xll.og.Swap.resolve(C5,C2)</f>
-        <v>ResolvedSwap@30</v>
+        <v>ResolvedSwap@14</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F3" s="20" t="str">
         <f>_xll.og.DiscountingSwapProductPricer.presentValueMultiCurrency(F2,C3,'Market Data'!B2)</f>
-        <v>MultiCurrencyAmount@31</v>
+        <v>MultiCurrencyAmount@16</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.45">
@@ -1558,7 +1558,7 @@
       </c>
       <c r="C5" s="8" t="str">
         <f>_xll.og.Swap.of(C6:C7)</f>
-        <v>Swap@30</v>
+        <v>Swap@18</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.45">
@@ -1567,7 +1567,7 @@
       </c>
       <c r="C6" s="1" t="str">
         <f>C9</f>
-        <v>RateCalculationSwapLeg@34</v>
+        <v>RateCalculationSwapLeg@19</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.45">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="C7" s="1" t="str">
         <f>H9</f>
-        <v>RateCalculationSwapLeg@18</v>
+        <v>RateCalculationSwapLeg@1</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.45">
@@ -1585,14 +1585,14 @@
       </c>
       <c r="C9" s="8" t="str">
         <f>_xll.og.RateCalculationSwapLeg.build(B10:B14,C10:C14)</f>
-        <v>RateCalculationSwapLeg@34</v>
+        <v>RateCalculationSwapLeg@19</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="8" t="str">
         <f>_xll.og.RateCalculationSwapLeg.build(G10:G14,H10:H14)</f>
-        <v>RateCalculationSwapLeg@18</v>
+        <v>RateCalculationSwapLeg@1</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.45">
@@ -1615,14 +1615,14 @@
       </c>
       <c r="C11" s="1" t="str">
         <f>C16</f>
-        <v>PeriodicSchedule@8</v>
+        <v>PeriodicSchedule@10</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H11" s="1" t="str">
         <f>H16</f>
-        <v>PeriodicSchedule@7</v>
+        <v>PeriodicSchedule@1</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.45">
@@ -1631,14 +1631,14 @@
       </c>
       <c r="C12" s="1" t="str">
         <f>C22</f>
-        <v>PaymentSchedule@7</v>
+        <v>PaymentSchedule@6</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="1" t="str">
         <f>H22</f>
-        <v>PaymentSchedule@8</v>
+        <v>PaymentSchedule@1</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.45">
@@ -1647,14 +1647,14 @@
       </c>
       <c r="C13" s="1" t="str">
         <f>_xll.og.NotionalSchedule.build(B27:B28,C27:C28)</f>
-        <v>NotionalSchedule@38</v>
+        <v>NotionalSchedule@3</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="1" t="str">
         <f>H26</f>
-        <v>NotionalSchedule@26</v>
+        <v>NotionalSchedule@2</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.45">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C14" s="1" t="str">
         <f>_xll.og.FixedRateCalculation.of(D14,E14)</f>
-        <v>FixedRateCalculation@14</v>
+        <v>FixedRateCalculation@6</v>
       </c>
       <c r="D14" s="7">
         <v>0.01</v>
@@ -1676,7 +1676,7 @@
       </c>
       <c r="H14" s="1" t="str">
         <f>_xll.og.IborRateCalculation.of(I14)</f>
-        <v>IborRateCalculation@4</v>
+        <v>IborRateCalculation@1</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>71</v>
@@ -1688,14 +1688,14 @@
       </c>
       <c r="C16" s="8" t="str">
         <f>_xll.og.PeriodicSchedule.build(B17:B20,C17:C20)</f>
-        <v>PeriodicSchedule@8</v>
+        <v>PeriodicSchedule@10</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="8" t="str">
         <f>_xll.og.PeriodicSchedule.build(G17:G20,H17:H20)</f>
-        <v>PeriodicSchedule@7</v>
+        <v>PeriodicSchedule@1</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.45">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="C20" s="1" t="str">
         <f>_xll.og.BusinessDayAdjustment.of(D20,E20)</f>
-        <v>BusinessDayAdjustment@8</v>
+        <v>BusinessDayAdjustment@1</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>7</v>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="H20" s="1" t="str">
         <f>_xll.og.BusinessDayAdjustment.of(I20,J20)</f>
-        <v>BusinessDayAdjustment@7</v>
+        <v>BusinessDayAdjustment@2</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>7</v>
@@ -1774,14 +1774,14 @@
       </c>
       <c r="C22" s="8" t="str">
         <f>_xll.og.PaymentSchedule.build(B23:B24,C23:C24)</f>
-        <v>PaymentSchedule@7</v>
+        <v>PaymentSchedule@6</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H22" s="8" t="str">
         <f>_xll.og.PaymentSchedule.build(G23:G24,H23:H24)</f>
-        <v>PaymentSchedule@8</v>
+        <v>PaymentSchedule@1</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.45">
@@ -1818,14 +1818,14 @@
       </c>
       <c r="C26" s="8" t="str">
         <f>_xll.og.NotionalSchedule.build(B27:B28,C27:C28)</f>
-        <v>NotionalSchedule@37</v>
+        <v>NotionalSchedule@1</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H26" s="8" t="str">
         <f>_xll.og.NotionalSchedule.build(G27:G28,H27:H28)</f>
-        <v>NotionalSchedule@26</v>
+        <v>NotionalSchedule@2</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Add Excel wrappers for more products and curve node types
Added:
  - IborFixingDeposit
  - TermDeposit
  - Fra
  - FxNdf
  - FxSingle
  - FxSwap
  - IborFuture
  - FixedInflationSwap
  - FixedRateSwapLeg
  - IborIborSwap
  - InflationRateSwapLeg
  - OvernightIborSwap
  - ThreeLegBasisSwap
  - XCcyIborIborSwap
</commit_message>
<xml_diff>
--- a/examples/swap-pricer.xlsx
+++ b/examples/swap-pricer.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="86">
   <si>
     <t>PayReceive</t>
   </si>
@@ -262,6 +262,27 @@
   </si>
   <si>
     <t>PV (EUR)</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>EUR-EURIBOR-6M</t>
+  </si>
+  <si>
+    <t>EUR-FIXED-1Y-EURIBOR-6M</t>
+  </si>
+  <si>
+    <t>EUR-EURIBOR-6M-IRS</t>
   </si>
 </sst>
 </file>
@@ -748,31 +769,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L41"/>
+  <dimension ref="B2:R43"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.19921875" customWidth="1"/>
-    <col min="2" max="4" width="33.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="33.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.46484375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.9296875" customWidth="1"/>
     <col min="8" max="8" width="33.796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="str">
         <f>_xll.og.CurveCalibrator.calibrate(_xll.og.CurveCalibrator.standard(),B8,C4,C6)</f>
-        <v>ImmutableRatesProvider@3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.45">
+        <v>ImmutableRatesProvider@10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>67</v>
       </c>
@@ -780,44 +805,48 @@
         <v>42429</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="17" t="str">
-        <f>_xll.og.MarketData.combinedWith(C5,D5)</f>
-        <v>ImmutableMarketData@7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+        <f>_xll.og.MarketData.combinedWith(_xll.og.MarketData.combinedWith(C5,D5),E5)</f>
+        <v>ImmutableMarketData@161</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C5" s="12" t="str">
         <f>_xll.og.MarketData.of(C3,E14:E27,D14:D27)</f>
-        <v>ImmutableMarketData@6</v>
+        <v>ImmutableMarketData@159</v>
       </c>
       <c r="D5" s="12" t="str">
-        <f>_xll.og.MarketData.of(C3,K14:K23,J14:J23)</f>
-        <v>ImmutableMarketData@1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
+        <f>_xll.og.MarketData.of(C3,K14:K26,J14:J26)</f>
+        <v>ImmutableMarketData@158</v>
+      </c>
+      <c r="E5" s="12" t="str">
+        <f>_xll.og.MarketData.of(C3,Q14:Q25,P14:P25)</f>
+        <v>ImmutableMarketData@157</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="12" t="str">
         <f>_xll.og.ReferenceData.standard()</f>
-        <v>ImmutableReferenceData@1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
+        <v>ImmutableReferenceData@23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B8" s="16" t="str">
-        <f>_xll.og.CurveGroupDefinition.of(C9,C10:D10,C11:D11)</f>
-        <v>CurveGroupDefinition@1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+        <f>_xll.og.CurveGroupDefinition.of(C9,C10:E10,C11:E11)</f>
+        <v>CurveGroupDefinition@44</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>48</v>
       </c>
@@ -825,33 +854,41 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="12" t="str">
-        <f>B38</f>
-        <v>CurveGroupEntry@2</v>
+        <f>B40</f>
+        <v>CurveGroupEntry@43</v>
       </c>
       <c r="D10" s="12" t="str">
-        <f>H38</f>
-        <v>CurveGroupEntry@1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+        <f>H40</f>
+        <v>CurveGroupEntry@42</v>
+      </c>
+      <c r="E10" s="12" t="str">
+        <f>N40</f>
+        <v>CurveGroupEntry@41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C11" s="12" t="str">
-        <f>B29</f>
-        <v>InterpolatedNodalCurveDefinition@2</v>
+        <f>B31</f>
+        <v>InterpolatedNodalCurveDefinition@68</v>
       </c>
       <c r="D11" s="12" t="str">
-        <f>H29</f>
-        <v>InterpolatedNodalCurveDefinition@1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
+        <f>H31</f>
+        <v>InterpolatedNodalCurveDefinition@67</v>
+      </c>
+      <c r="E11" s="12" t="str">
+        <f>N31</f>
+        <v>InterpolatedNodalCurveDefinition@66</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
@@ -882,8 +919,23 @@
       <c r="L13" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="N13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B14" s="12" t="s">
         <v>29</v>
       </c>
@@ -895,31 +947,44 @@
       </c>
       <c r="E14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B14&amp;"."&amp;C14)</f>
-        <v>QuoteId@22</v>
+        <v>QuoteId@616</v>
       </c>
       <c r="F14" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C14,B14),E14)</f>
-        <v>FixedOvernightSwapCurveNode@14</v>
+        <v>FixedOvernightSwapCurveNode@252</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>30</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="I14" s="12"/>
       <c r="J14" s="18">
-        <v>-3.15E-3</v>
+        <v>-2.0500000000000002E-3</v>
       </c>
       <c r="K14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H14&amp;"."&amp;I14)</f>
-        <v>QuoteId@10</v>
+        <v>QuoteId@593</v>
       </c>
       <c r="L14" s="13" t="str">
-        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I14,H14),K14)</f>
-        <v>FixedIborSwapCurveNode@10</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
+        <f>_xll.og.IborFixingDepositCurveNode.ofRate( _xll.og.IborFixingDepositTemplate.of(H14),K14)</f>
+        <v>IborFixingDepositCurveNode@28</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="O14" s="12"/>
+      <c r="P14" s="18">
+        <v>-1.34E-3</v>
+      </c>
+      <c r="Q14" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;N14&amp;"."&amp;O14)</f>
+        <v>QuoteId@587</v>
+      </c>
+      <c r="R14" s="13" t="str">
+        <f>_xll.og.IborFixingDepositCurveNode.ofRate( _xll.og.IborFixingDepositTemplate.of(N14),Q14)</f>
+        <v>IborFixingDepositCurveNode@27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B15" s="12" t="s">
         <v>29</v>
       </c>
@@ -931,31 +996,48 @@
       </c>
       <c r="E15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B15&amp;"."&amp;C15)</f>
-        <v>QuoteId@12</v>
+        <v>QuoteId@603</v>
       </c>
       <c r="F15" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C15,B15),E15)</f>
-        <v>FixedOvernightSwapCurveNode@4</v>
+        <v>FixedOvernightSwapCurveNode@241</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J15" s="18">
-        <v>-3.4499999999999999E-3</v>
+        <v>-3.0999999999999999E-3</v>
       </c>
       <c r="K15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H15&amp;"."&amp;I15)</f>
-        <v>QuoteId@9</v>
+        <v>QuoteId@591</v>
       </c>
       <c r="L15" s="13" t="str">
-        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I15,H15),K15)</f>
-        <v>FixedIborSwapCurveNode@9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+        <f>_xll.og.FraCurveNode.ofRate(_xll.og.FraTemplate.ofIndex(I15,H15),K15)</f>
+        <v>FraCurveNode@38</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="P15" s="18">
+        <v>-2.15E-3</v>
+      </c>
+      <c r="Q15" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;N15&amp;"."&amp;O15)</f>
+        <v>QuoteId@584</v>
+      </c>
+      <c r="R15" s="13" t="str">
+        <f>_xll.og.FraCurveNode.ofRate(_xll.og.FraTemplate.ofIndex(O15,N15),Q15)</f>
+        <v>FraCurveNode@36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B16" s="12" t="s">
         <v>29</v>
       </c>
@@ -967,31 +1049,48 @@
       </c>
       <c r="E16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B16&amp;"."&amp;C16)</f>
-        <v>QuoteId@11</v>
+        <v>QuoteId@604</v>
       </c>
       <c r="F16" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C16,B16),E16)</f>
-        <v>FixedOvernightSwapCurveNode@1</v>
+        <v>FixedOvernightSwapCurveNode@239</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J16" s="18">
-        <v>-3.1999999999999997E-3</v>
+        <v>-3.0999999999999999E-3</v>
       </c>
       <c r="K16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H16&amp;"."&amp;I16)</f>
-        <v>QuoteId@5</v>
+        <v>QuoteId@590</v>
       </c>
       <c r="L16" s="13" t="str">
-        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I16,H16),K16)</f>
-        <v>FixedIborSwapCurveNode@7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.45">
+        <f>_xll.og.FraCurveNode.ofRate(_xll.og.FraTemplate.ofIndex(I16,H16),K16)</f>
+        <v>FraCurveNode@37</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" s="18">
+        <v>-1.9E-3</v>
+      </c>
+      <c r="Q16" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;N16&amp;"."&amp;O16)</f>
+        <v>QuoteId@586</v>
+      </c>
+      <c r="R16" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O16,N16),Q16)</f>
+        <v>FixedIborSwapCurveNode@250</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B17" s="12" t="s">
         <v>29</v>
       </c>
@@ -1003,31 +1102,48 @@
       </c>
       <c r="E17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B17&amp;"."&amp;C17)</f>
-        <v>QuoteId@13</v>
+        <v>QuoteId@606</v>
       </c>
       <c r="F17" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C17,B17),E17)</f>
-        <v>FixedOvernightSwapCurveNode@2</v>
+        <v>FixedOvernightSwapCurveNode@242</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>75</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="J17" s="18">
-        <v>-2.4999999999999996E-3</v>
+        <v>-3.15E-3</v>
       </c>
       <c r="K17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H17&amp;"."&amp;I17)</f>
-        <v>QuoteId@6</v>
+        <v>QuoteId@592</v>
       </c>
       <c r="L17" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I17,H17),K17)</f>
-        <v>FixedIborSwapCurveNode@5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@254</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="P17" s="18">
+        <v>-2.2000000000000001E-3</v>
+      </c>
+      <c r="Q17" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;N17&amp;"."&amp;O17)</f>
+        <v>QuoteId@589</v>
+      </c>
+      <c r="R17" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O17,N17),Q17)</f>
+        <v>FixedIborSwapCurveNode@253</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B18" s="12" t="s">
         <v>29</v>
       </c>
@@ -1039,31 +1155,48 @@
       </c>
       <c r="E18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B18&amp;"."&amp;C18)</f>
-        <v>QuoteId@14</v>
+        <v>QuoteId@605</v>
       </c>
       <c r="F18" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C18,B18),E18)</f>
-        <v>FixedOvernightSwapCurveNode@3</v>
+        <v>FixedOvernightSwapCurveNode@240</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>75</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J18" s="18">
-        <v>-1.6750000000000001E-3</v>
+        <v>-3.4499999999999999E-3</v>
       </c>
       <c r="K18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H18&amp;"."&amp;I18)</f>
-        <v>QuoteId@8</v>
+        <v>QuoteId@601</v>
       </c>
       <c r="L18" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I18,H18),K18)</f>
-        <v>FixedIborSwapCurveNode@8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@263</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="P18" s="18">
+        <v>-1.9E-3</v>
+      </c>
+      <c r="Q18" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;N18&amp;"."&amp;O18)</f>
+        <v>QuoteId@585</v>
+      </c>
+      <c r="R18" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O18,N18),Q18)</f>
+        <v>FixedIborSwapCurveNode@249</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B19" s="12" t="s">
         <v>29</v>
       </c>
@@ -1075,31 +1208,48 @@
       </c>
       <c r="E19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B19&amp;"."&amp;C19)</f>
-        <v>QuoteId@15</v>
+        <v>QuoteId@609</v>
       </c>
       <c r="F19" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C19,B19),E19)</f>
-        <v>FixedOvernightSwapCurveNode@6</v>
+        <v>FixedOvernightSwapCurveNode@244</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>75</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J19" s="18">
-        <v>5.4999999999999992E-4</v>
+        <v>-3.1999999999999997E-3</v>
       </c>
       <c r="K19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H19&amp;"."&amp;I19)</f>
-        <v>QuoteId@7</v>
+        <v>QuoteId@599</v>
       </c>
       <c r="L19" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I19,H19),K19)</f>
-        <v>FixedIborSwapCurveNode@6</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@258</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="P19" s="18">
+        <v>-1.1999999999999999E-3</v>
+      </c>
+      <c r="Q19" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;N19&amp;"."&amp;O19)</f>
+        <v>QuoteId@583</v>
+      </c>
+      <c r="R19" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O19,N19),Q19)</f>
+        <v>FixedIborSwapCurveNode@248</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B20" s="12" t="s">
         <v>29</v>
       </c>
@@ -1111,31 +1261,48 @@
       </c>
       <c r="E20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B20&amp;"."&amp;C20)</f>
-        <v>QuoteId@16</v>
+        <v>QuoteId@607</v>
       </c>
       <c r="F20" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C20,B20),E20)</f>
-        <v>FixedOvernightSwapCurveNode@5</v>
+        <v>FixedOvernightSwapCurveNode@249</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>75</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J20" s="18">
-        <v>3.8999999999999998E-3</v>
+        <v>-2.4999999999999996E-3</v>
       </c>
       <c r="K20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H20&amp;"."&amp;I20)</f>
-        <v>QuoteId@3</v>
+        <v>QuoteId@597</v>
       </c>
       <c r="L20" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I20,H20),K20)</f>
-        <v>FixedIborSwapCurveNode@3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@260</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="P20" s="18">
+        <v>-3.2499999999999999E-4</v>
+      </c>
+      <c r="Q20" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;N20&amp;"."&amp;O20)</f>
+        <v>QuoteId@588</v>
+      </c>
+      <c r="R20" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O20,N20),Q20)</f>
+        <v>FixedIborSwapCurveNode@251</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B21" s="12" t="s">
         <v>29</v>
       </c>
@@ -1147,31 +1314,48 @@
       </c>
       <c r="E21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B21&amp;"."&amp;C21)</f>
-        <v>QuoteId@20</v>
+        <v>QuoteId@610</v>
       </c>
       <c r="F21" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C21,B21),E21)</f>
-        <v>FixedOvernightSwapCurveNode@13</v>
+        <v>FixedOvernightSwapCurveNode@245</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>75</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J21" s="18">
-        <v>7.4000000000000003E-3</v>
+        <v>-1.6750000000000001E-3</v>
       </c>
       <c r="K21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H21&amp;"."&amp;I21)</f>
-        <v>QuoteId@2</v>
+        <v>QuoteId@598</v>
       </c>
       <c r="L21" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I21,H21),K21)</f>
-        <v>FixedIborSwapCurveNode@4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@257</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="P21" s="18">
+        <v>1.8E-3</v>
+      </c>
+      <c r="Q21" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;N21&amp;"."&amp;O21)</f>
+        <v>QuoteId@582</v>
+      </c>
+      <c r="R21" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O21,N21),Q21)</f>
+        <v>FixedIborSwapCurveNode@246</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B22" s="12" t="s">
         <v>29</v>
       </c>
@@ -1183,31 +1367,48 @@
       </c>
       <c r="E22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B22&amp;"."&amp;C22)</f>
-        <v>QuoteId@17</v>
+        <v>QuoteId@608</v>
       </c>
       <c r="F22" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C22,B22),E22)</f>
-        <v>FixedOvernightSwapCurveNode@7</v>
+        <v>FixedOvernightSwapCurveNode@243</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>75</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J22" s="18">
-        <v>8.8000000000000005E-3</v>
+        <v>5.4999999999999992E-4</v>
       </c>
       <c r="K22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H22&amp;"."&amp;I22)</f>
-        <v>QuoteId@4</v>
+        <v>QuoteId@600</v>
       </c>
       <c r="L22" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I22,H22),K22)</f>
-        <v>FixedIborSwapCurveNode@1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@261</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O22" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="P22" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="Q22" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;N22&amp;"."&amp;O22)</f>
+        <v>QuoteId@581</v>
+      </c>
+      <c r="R22" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O22,N22),Q22)</f>
+        <v>FixedIborSwapCurveNode@245</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B23" s="12" t="s">
         <v>29</v>
       </c>
@@ -1219,31 +1420,48 @@
       </c>
       <c r="E23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B23&amp;"."&amp;C23)</f>
-        <v>QuoteId@18</v>
+        <v>QuoteId@612</v>
       </c>
       <c r="F23" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C23,B23),E23)</f>
-        <v>FixedOvernightSwapCurveNode@12</v>
+        <v>FixedOvernightSwapCurveNode@248</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>75</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J23" s="18">
-        <v>9.4999999999999998E-3</v>
+        <v>3.8999999999999998E-3</v>
       </c>
       <c r="K23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H23&amp;"."&amp;I23)</f>
-        <v>QuoteId@1</v>
+        <v>QuoteId@595</v>
       </c>
       <c r="L23" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I23,H23),K23)</f>
-        <v>FixedIborSwapCurveNode@2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@259</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="P23" s="18">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="Q23" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;N23&amp;"."&amp;O23)</f>
+        <v>QuoteId@580</v>
+      </c>
+      <c r="R23" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O23,N23),Q23)</f>
+        <v>FixedIborSwapCurveNode@247</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B24" s="12" t="s">
         <v>29</v>
       </c>
@@ -1255,14 +1473,48 @@
       </c>
       <c r="E24" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B24&amp;"."&amp;C24)</f>
-        <v>QuoteId@19</v>
+        <v>QuoteId@615</v>
       </c>
       <c r="F24" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C24,B24),E24)</f>
-        <v>FixedOvernightSwapCurveNode@9</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
+        <v>FixedOvernightSwapCurveNode@251</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J24" s="18">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="K24" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;H24&amp;"."&amp;I24)</f>
+        <v>QuoteId@594</v>
+      </c>
+      <c r="L24" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I24,H24),K24)</f>
+        <v>FixedIborSwapCurveNode@255</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O24" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="P24" s="18">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="Q24" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;N24&amp;"."&amp;O24)</f>
+        <v>QuoteId@578</v>
+      </c>
+      <c r="R24" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O24,N24),Q24)</f>
+        <v>FixedIborSwapCurveNode@252</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B25" s="12" t="s">
         <v>29</v>
       </c>
@@ -1274,14 +1526,48 @@
       </c>
       <c r="E25" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B25&amp;"."&amp;C25)</f>
-        <v>QuoteId@24</v>
+        <v>QuoteId@613</v>
       </c>
       <c r="F25" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C25,B25),E25)</f>
-        <v>FixedOvernightSwapCurveNode@11</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.45">
+        <v>FixedOvernightSwapCurveNode@247</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="18">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="K25" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;H25&amp;"."&amp;I25)</f>
+        <v>QuoteId@596</v>
+      </c>
+      <c r="L25" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I25,H25),K25)</f>
+        <v>FixedIborSwapCurveNode@256</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="P25" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="Q25" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;N25&amp;"."&amp;O25)</f>
+        <v>QuoteId@579</v>
+      </c>
+      <c r="R25" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O25,N25),Q25)</f>
+        <v>FixedIborSwapCurveNode@244</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B26" s="12" t="s">
         <v>29</v>
       </c>
@@ -1293,14 +1579,31 @@
       </c>
       <c r="E26" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B26&amp;"."&amp;C26)</f>
-        <v>QuoteId@21</v>
+        <v>QuoteId@611</v>
       </c>
       <c r="F26" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C26,B26),E26)</f>
-        <v>FixedOvernightSwapCurveNode@8</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.45">
+        <v>FixedOvernightSwapCurveNode@246</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J26" s="18">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="K26" s="13" t="str">
+        <f>_xll.og.QuoteId.of("Excel~" &amp;H26&amp;"."&amp;I26)</f>
+        <v>QuoteId@602</v>
+      </c>
+      <c r="L26" s="13" t="str">
+        <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I26,H26),K26)</f>
+        <v>FixedIborSwapCurveNode@262</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B27" s="12" t="s">
         <v>29</v>
       </c>
@@ -1312,179 +1615,251 @@
       </c>
       <c r="E27" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B27&amp;"."&amp;C27)</f>
-        <v>QuoteId@23</v>
+        <v>QuoteId@614</v>
       </c>
       <c r="F27" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C27,B27),E27)</f>
-        <v>FixedOvernightSwapCurveNode@10</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B29" s="16" t="str">
-        <f>_xll.og.InterpolatedNodalCurveDefinition.build(B30:B36,C30:C36,F14:F27)</f>
-        <v>InterpolatedNodalCurveDefinition@2</v>
-      </c>
-      <c r="H29" s="16" t="str">
-        <f>_xll.og.InterpolatedNodalCurveDefinition.build(H30:H36,I30:I36,L14:L23)</f>
-        <v>InterpolatedNodalCurveDefinition@1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B30" s="2" t="s">
+        <v>FixedOvernightSwapCurveNode@250</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B31" s="16" t="str">
+        <f>_xll.og.InterpolatedNodalCurveDefinition.build(B32:B38,C32:C38,F14:F27)</f>
+        <v>InterpolatedNodalCurveDefinition@68</v>
+      </c>
+      <c r="H31" s="16" t="str">
+        <f>_xll.og.InterpolatedNodalCurveDefinition.build(H32:H38,I32:I38,L14:L26)</f>
+        <v>InterpolatedNodalCurveDefinition@67</v>
+      </c>
+      <c r="N31" s="16" t="str">
+        <f>_xll.og.InterpolatedNodalCurveDefinition.build(N32:N38,O32:O38,R14:R25)</f>
+        <v>InterpolatedNodalCurveDefinition@66</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B32" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C32" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I30" s="12" t="s">
+      <c r="I32" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B31" s="2" t="s">
+      <c r="N32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O32" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B33" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C33" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I31" s="12" t="s">
+      <c r="I33" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B32" s="2" t="s">
+      <c r="N33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O33" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C34" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I32" s="12" t="s">
+      <c r="I34" s="12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B33" s="2" t="s">
+      <c r="N34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O34" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B35" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C35" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I33" s="12" t="s">
+      <c r="I35" s="12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B34" s="2" t="s">
+      <c r="N35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O35" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B36" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C36" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I34" s="12" t="s">
+      <c r="I36" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B35" s="2" t="s">
+      <c r="N36" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O36" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B37" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I35" s="12" t="s">
+      <c r="I37" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B36" s="2" t="s">
+      <c r="N37" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O37" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B38" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C38" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I36" s="12" t="s">
+      <c r="I38" s="12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B38" s="16" t="str">
-        <f>_xll.og.CurveGroupEntry.of(C39,C40,C41)</f>
-        <v>CurveGroupEntry@2</v>
-      </c>
-      <c r="H38" s="16" t="str">
-        <f>_xll.og.CurveGroupEntry.of(I39,I40,I41)</f>
-        <v>CurveGroupEntry@1</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B39" s="2" t="s">
+      <c r="N38" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O38" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B40" s="16" t="str">
+        <f>_xll.og.CurveGroupEntry.of(C41,C42,C43)</f>
+        <v>CurveGroupEntry@43</v>
+      </c>
+      <c r="H40" s="16" t="str">
+        <f>_xll.og.CurveGroupEntry.of(I41,I42,I43)</f>
+        <v>CurveGroupEntry@42</v>
+      </c>
+      <c r="N40" s="16" t="str">
+        <f>_xll.og.CurveGroupEntry.of(O41,O42,O43)</f>
+        <v>CurveGroupEntry@41</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B41" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C41" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I39" s="12" t="s">
+      <c r="I41" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B40" s="2" t="s">
+      <c r="N41" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O41" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B42" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C42" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I40" s="12" t="s">
+      <c r="I42" s="12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B41" s="2" t="s">
+      <c r="N42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O42" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B43" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="12" t="str">
-        <f>_xll.og.OvernightIndex.of(D41)</f>
-        <v>ImmutableOvernightIndex@1</v>
-      </c>
-      <c r="D41" s="4" t="s">
+      <c r="C43" s="12" t="str">
+        <f>_xll.og.OvernightIndex.of(D43)</f>
+        <v>ImmutableOvernightIndex@14</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I41" s="12" t="str">
-        <f>_xll.og.IborIndex.of(J41)</f>
-        <v>ImmutableIborIndex@1</v>
-      </c>
-      <c r="J41" s="4" t="s">
+      <c r="I43" s="12" t="str">
+        <f>_xll.og.IborIndex.of(J43)</f>
+        <v>ImmutableIborIndex@28</v>
+      </c>
+      <c r="J43" s="4" t="s">
         <v>71</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O43" s="12" t="str">
+        <f>_xll.og.IborIndex.of(P43)</f>
+        <v>ImmutableIborIndex@27</v>
+      </c>
+      <c r="P43" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1517,14 +1892,14 @@
       </c>
       <c r="C2" s="8" t="str">
         <f>_xll.og.ReferenceData.standard()</f>
-        <v>ImmutableReferenceData@2</v>
+        <v>ImmutableReferenceData@24</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>69</v>
       </c>
       <c r="F2" s="20" t="str">
         <f>_xll.og.DiscountingSwapProductPricer.DEFAULT()</f>
-        <v>DiscountingSwapProductPricer@1</v>
+        <v>DiscountingSwapProductPricer@10</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.45">
@@ -1533,14 +1908,14 @@
       </c>
       <c r="C3" s="8" t="str">
         <f>_xll.og.Swap.resolve(C5,C2)</f>
-        <v>ResolvedSwap@14</v>
+        <v>ResolvedSwap@10</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F3" s="20" t="str">
         <f>_xll.og.DiscountingSwapProductPricer.presentValueMultiCurrency(F2,C3,'Market Data'!B2)</f>
-        <v>MultiCurrencyAmount@16</v>
+        <v>MultiCurrencyAmount@5</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.45">
@@ -1549,7 +1924,7 @@
       </c>
       <c r="F4" s="21">
         <f>_xll.og.CurrencyAmount.getAmount(_xll.og.MultiCurrencyAmount.getAmountOrZero(F3,"EUR"))</f>
-        <v>-272886.3740554215</v>
+        <v>-272455.95127698663</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.45">
@@ -1558,7 +1933,7 @@
       </c>
       <c r="C5" s="8" t="str">
         <f>_xll.og.Swap.of(C6:C7)</f>
-        <v>Swap@18</v>
+        <v>Swap@10</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.45">
@@ -1567,7 +1942,7 @@
       </c>
       <c r="C6" s="1" t="str">
         <f>C9</f>
-        <v>RateCalculationSwapLeg@19</v>
+        <v>RateCalculationSwapLeg@20</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.45">
@@ -1576,7 +1951,7 @@
       </c>
       <c r="C7" s="1" t="str">
         <f>H9</f>
-        <v>RateCalculationSwapLeg@1</v>
+        <v>RateCalculationSwapLeg@19</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.45">
@@ -1585,14 +1960,14 @@
       </c>
       <c r="C9" s="8" t="str">
         <f>_xll.og.RateCalculationSwapLeg.build(B10:B14,C10:C14)</f>
-        <v>RateCalculationSwapLeg@19</v>
+        <v>RateCalculationSwapLeg@20</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="8" t="str">
         <f>_xll.og.RateCalculationSwapLeg.build(G10:G14,H10:H14)</f>
-        <v>RateCalculationSwapLeg@1</v>
+        <v>RateCalculationSwapLeg@19</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.45">
@@ -1615,14 +1990,14 @@
       </c>
       <c r="C11" s="1" t="str">
         <f>C16</f>
-        <v>PeriodicSchedule@10</v>
+        <v>PeriodicSchedule@20</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H11" s="1" t="str">
         <f>H16</f>
-        <v>PeriodicSchedule@1</v>
+        <v>PeriodicSchedule@19</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.45">
@@ -1631,14 +2006,14 @@
       </c>
       <c r="C12" s="1" t="str">
         <f>C22</f>
-        <v>PaymentSchedule@6</v>
+        <v>PaymentSchedule@20</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="1" t="str">
         <f>H22</f>
-        <v>PaymentSchedule@1</v>
+        <v>PaymentSchedule@19</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.45">
@@ -1647,14 +2022,14 @@
       </c>
       <c r="C13" s="1" t="str">
         <f>_xll.og.NotionalSchedule.build(B27:B28,C27:C28)</f>
-        <v>NotionalSchedule@3</v>
+        <v>NotionalSchedule@30</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="1" t="str">
         <f>H26</f>
-        <v>NotionalSchedule@2</v>
+        <v>NotionalSchedule@28</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.45">
@@ -1663,7 +2038,7 @@
       </c>
       <c r="C14" s="1" t="str">
         <f>_xll.og.FixedRateCalculation.of(D14,E14)</f>
-        <v>FixedRateCalculation@6</v>
+        <v>FixedRateCalculation@10</v>
       </c>
       <c r="D14" s="7">
         <v>0.01</v>
@@ -1676,7 +2051,7 @@
       </c>
       <c r="H14" s="1" t="str">
         <f>_xll.og.IborRateCalculation.of(I14)</f>
-        <v>IborRateCalculation@1</v>
+        <v>IborRateCalculation@10</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>71</v>
@@ -1688,14 +2063,14 @@
       </c>
       <c r="C16" s="8" t="str">
         <f>_xll.og.PeriodicSchedule.build(B17:B20,C17:C20)</f>
-        <v>PeriodicSchedule@10</v>
+        <v>PeriodicSchedule@20</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="8" t="str">
         <f>_xll.og.PeriodicSchedule.build(G17:G20,H17:H20)</f>
-        <v>PeriodicSchedule@1</v>
+        <v>PeriodicSchedule@19</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.45">
@@ -1746,7 +2121,7 @@
       </c>
       <c r="C20" s="1" t="str">
         <f>_xll.og.BusinessDayAdjustment.of(D20,E20)</f>
-        <v>BusinessDayAdjustment@1</v>
+        <v>BusinessDayAdjustment@20</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>7</v>
@@ -1759,7 +2134,7 @@
       </c>
       <c r="H20" s="1" t="str">
         <f>_xll.og.BusinessDayAdjustment.of(I20,J20)</f>
-        <v>BusinessDayAdjustment@2</v>
+        <v>BusinessDayAdjustment@19</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>7</v>
@@ -1774,14 +2149,14 @@
       </c>
       <c r="C22" s="8" t="str">
         <f>_xll.og.PaymentSchedule.build(B23:B24,C23:C24)</f>
-        <v>PaymentSchedule@6</v>
+        <v>PaymentSchedule@20</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H22" s="8" t="str">
         <f>_xll.og.PaymentSchedule.build(G23:G24,H23:H24)</f>
-        <v>PaymentSchedule@1</v>
+        <v>PaymentSchedule@19</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.45">
@@ -1818,14 +2193,14 @@
       </c>
       <c r="C26" s="8" t="str">
         <f>_xll.og.NotionalSchedule.build(B27:B28,C27:C28)</f>
-        <v>NotionalSchedule@1</v>
+        <v>NotionalSchedule@29</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H26" s="8" t="str">
         <f>_xll.og.NotionalSchedule.build(G27:G28,H27:H28)</f>
-        <v>NotionalSchedule@2</v>
+        <v>NotionalSchedule@28</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Add swap sensitivities and some util functions
- Added util functions for expanding objects
    - og.Object.toString
    - og.List.explode
    - og.List.size
    - og.List.get
    - og.Bean.expode
    - og.Bean.property
    - og.Bean.propertyNames

- Moved generated code out into sub-package to keep it clear whats generated
  hand coded classes.

- Use @ExcelReturnConverter to convert Java objects to strings on
  returning to Excel where possible.
</commit_message>
<xml_diff>
--- a/examples/swap-pricer.xlsx
+++ b/examples/swap-pricer.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="88">
   <si>
     <t>PayReceive</t>
   </si>
@@ -264,18 +264,6 @@
     <t>PV (EUR)</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>EUR-EURIBOR-6M</t>
   </si>
   <si>
@@ -283,6 +271,24 @@
   </si>
   <si>
     <t>EUR-EURIBOR-6M-IRS</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>yearFraction</t>
+  </si>
+  <si>
+    <t>sensitivity</t>
+  </si>
+  <si>
+    <t>observation.index.name</t>
+  </si>
+  <si>
+    <t>observation.yearFraction</t>
+  </si>
+  <si>
+    <t>Sensitivities</t>
   </si>
 </sst>
 </file>
@@ -430,7 +436,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -453,6 +459,10 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="3" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -771,7 +781,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R43"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -794,7 +806,7 @@
     <row r="2" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="str">
         <f>_xll.og.CurveCalibrator.calibrate(_xll.og.CurveCalibrator.standard(),B8,C4,C6)</f>
-        <v>ImmutableRatesProvider@10</v>
+        <v>ImmutableRatesProvider@1</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.45">
@@ -811,7 +823,7 @@
       </c>
       <c r="C4" s="17" t="str">
         <f>_xll.og.MarketData.combinedWith(_xll.og.MarketData.combinedWith(C5,D5),E5)</f>
-        <v>ImmutableMarketData@161</v>
+        <v>ImmutableMarketData@5</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -820,15 +832,15 @@
       </c>
       <c r="C5" s="12" t="str">
         <f>_xll.og.MarketData.of(C3,E14:E27,D14:D27)</f>
-        <v>ImmutableMarketData@159</v>
+        <v>ImmutableMarketData@1</v>
       </c>
       <c r="D5" s="12" t="str">
         <f>_xll.og.MarketData.of(C3,K14:K26,J14:J26)</f>
-        <v>ImmutableMarketData@158</v>
+        <v>ImmutableMarketData@3</v>
       </c>
       <c r="E5" s="12" t="str">
         <f>_xll.og.MarketData.of(C3,Q14:Q25,P14:P25)</f>
-        <v>ImmutableMarketData@157</v>
+        <v>ImmutableMarketData@2</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.45">
@@ -837,13 +849,13 @@
       </c>
       <c r="C6" s="12" t="str">
         <f>_xll.og.ReferenceData.standard()</f>
-        <v>ImmutableReferenceData@23</v>
+        <v>ImmutableReferenceData@2</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B8" s="16" t="str">
         <f>_xll.og.CurveGroupDefinition.of(C9,C10:E10,C11:E11)</f>
-        <v>CurveGroupDefinition@44</v>
+        <v>CurveGroupDefinition@1</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.45">
@@ -860,15 +872,15 @@
       </c>
       <c r="C10" s="12" t="str">
         <f>B40</f>
-        <v>CurveGroupEntry@43</v>
+        <v>CurveGroupEntry@1</v>
       </c>
       <c r="D10" s="12" t="str">
         <f>H40</f>
-        <v>CurveGroupEntry@42</v>
+        <v>CurveGroupEntry@3</v>
       </c>
       <c r="E10" s="12" t="str">
         <f>N40</f>
-        <v>CurveGroupEntry@41</v>
+        <v>CurveGroupEntry@2</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.45">
@@ -877,15 +889,15 @@
       </c>
       <c r="C11" s="12" t="str">
         <f>B31</f>
-        <v>InterpolatedNodalCurveDefinition@68</v>
+        <v>InterpolatedNodalCurveDefinition@2</v>
       </c>
       <c r="D11" s="12" t="str">
         <f>H31</f>
-        <v>InterpolatedNodalCurveDefinition@67</v>
+        <v>InterpolatedNodalCurveDefinition@3</v>
       </c>
       <c r="E11" s="12" t="str">
         <f>N31</f>
-        <v>InterpolatedNodalCurveDefinition@66</v>
+        <v>InterpolatedNodalCurveDefinition@1</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.45">
@@ -947,11 +959,11 @@
       </c>
       <c r="E14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B14&amp;"."&amp;C14)</f>
-        <v>QuoteId@616</v>
+        <v>QuoteId@7</v>
       </c>
       <c r="F14" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C14,B14),E14)</f>
-        <v>FixedOvernightSwapCurveNode@252</v>
+        <v>FixedOvernightSwapCurveNode@14</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>71</v>
@@ -962,14 +974,14 @@
       </c>
       <c r="K14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H14&amp;"."&amp;I14)</f>
-        <v>QuoteId@593</v>
+        <v>QuoteId@2</v>
       </c>
       <c r="L14" s="13" t="str">
         <f>_xll.og.IborFixingDepositCurveNode.ofRate( _xll.og.IborFixingDepositTemplate.of(H14),K14)</f>
-        <v>IborFixingDepositCurveNode@28</v>
+        <v>IborFixingDepositCurveNode@2</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="O14" s="12"/>
       <c r="P14" s="18">
@@ -977,11 +989,11 @@
       </c>
       <c r="Q14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N14&amp;"."&amp;O14)</f>
-        <v>QuoteId@587</v>
+        <v>QuoteId@1</v>
       </c>
       <c r="R14" s="13" t="str">
         <f>_xll.og.IborFixingDepositCurveNode.ofRate( _xll.og.IborFixingDepositTemplate.of(N14),Q14)</f>
-        <v>IborFixingDepositCurveNode@27</v>
+        <v>IborFixingDepositCurveNode@1</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.45">
@@ -996,11 +1008,11 @@
       </c>
       <c r="E15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B15&amp;"."&amp;C15)</f>
-        <v>QuoteId@603</v>
+        <v>QuoteId@5</v>
       </c>
       <c r="F15" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C15,B15),E15)</f>
-        <v>FixedOvernightSwapCurveNode@241</v>
+        <v>FixedOvernightSwapCurveNode@1</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>71</v>
@@ -1013,14 +1025,14 @@
       </c>
       <c r="K15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H15&amp;"."&amp;I15)</f>
-        <v>QuoteId@591</v>
+        <v>QuoteId@8</v>
       </c>
       <c r="L15" s="13" t="str">
         <f>_xll.og.FraCurveNode.ofRate(_xll.og.FraTemplate.ofIndex(I15,H15),K15)</f>
-        <v>FraCurveNode@38</v>
+        <v>FraCurveNode@2</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="O15" s="12" t="s">
         <v>37</v>
@@ -1030,11 +1042,11 @@
       </c>
       <c r="Q15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N15&amp;"."&amp;O15)</f>
-        <v>QuoteId@584</v>
+        <v>QuoteId@4</v>
       </c>
       <c r="R15" s="13" t="str">
         <f>_xll.og.FraCurveNode.ofRate(_xll.og.FraTemplate.ofIndex(O15,N15),Q15)</f>
-        <v>FraCurveNode@36</v>
+        <v>FraCurveNode@1</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.45">
@@ -1049,11 +1061,11 @@
       </c>
       <c r="E16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B16&amp;"."&amp;C16)</f>
-        <v>QuoteId@604</v>
+        <v>QuoteId@3</v>
       </c>
       <c r="F16" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C16,B16),E16)</f>
-        <v>FixedOvernightSwapCurveNode@239</v>
+        <v>FixedOvernightSwapCurveNode@3</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>71</v>
@@ -1066,14 +1078,14 @@
       </c>
       <c r="K16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H16&amp;"."&amp;I16)</f>
-        <v>QuoteId@590</v>
+        <v>QuoteId@10</v>
       </c>
       <c r="L16" s="13" t="str">
         <f>_xll.og.FraCurveNode.ofRate(_xll.og.FraTemplate.ofIndex(I16,H16),K16)</f>
-        <v>FraCurveNode@37</v>
+        <v>FraCurveNode@3</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="O16" s="12" t="s">
         <v>30</v>
@@ -1083,11 +1095,11 @@
       </c>
       <c r="Q16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N16&amp;"."&amp;O16)</f>
-        <v>QuoteId@586</v>
+        <v>QuoteId@9</v>
       </c>
       <c r="R16" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O16,N16),Q16)</f>
-        <v>FixedIborSwapCurveNode@250</v>
+        <v>FixedIborSwapCurveNode@4</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.45">
@@ -1102,11 +1114,11 @@
       </c>
       <c r="E17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B17&amp;"."&amp;C17)</f>
-        <v>QuoteId@606</v>
+        <v>QuoteId@6</v>
       </c>
       <c r="F17" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C17,B17),E17)</f>
-        <v>FixedOvernightSwapCurveNode@242</v>
+        <v>FixedOvernightSwapCurveNode@2</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>75</v>
@@ -1119,14 +1131,14 @@
       </c>
       <c r="K17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H17&amp;"."&amp;I17)</f>
-        <v>QuoteId@592</v>
+        <v>QuoteId@12</v>
       </c>
       <c r="L17" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I17,H17),K17)</f>
-        <v>FixedIborSwapCurveNode@254</v>
+        <v>FixedIborSwapCurveNode@3</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="O17" s="12" t="s">
         <v>39</v>
@@ -1136,11 +1148,11 @@
       </c>
       <c r="Q17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N17&amp;"."&amp;O17)</f>
-        <v>QuoteId@589</v>
+        <v>QuoteId@13</v>
       </c>
       <c r="R17" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O17,N17),Q17)</f>
-        <v>FixedIborSwapCurveNode@253</v>
+        <v>FixedIborSwapCurveNode@1</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.45">
@@ -1155,11 +1167,11 @@
       </c>
       <c r="E18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B18&amp;"."&amp;C18)</f>
-        <v>QuoteId@605</v>
+        <v>QuoteId@16</v>
       </c>
       <c r="F18" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C18,B18),E18)</f>
-        <v>FixedOvernightSwapCurveNode@240</v>
+        <v>FixedOvernightSwapCurveNode@5</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>75</v>
@@ -1172,14 +1184,14 @@
       </c>
       <c r="K18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H18&amp;"."&amp;I18)</f>
-        <v>QuoteId@601</v>
+        <v>QuoteId@11</v>
       </c>
       <c r="L18" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I18,H18),K18)</f>
-        <v>FixedIborSwapCurveNode@263</v>
+        <v>FixedIborSwapCurveNode@2</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="O18" s="12" t="s">
         <v>40</v>
@@ -1189,11 +1201,11 @@
       </c>
       <c r="Q18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N18&amp;"."&amp;O18)</f>
-        <v>QuoteId@585</v>
+        <v>QuoteId@14</v>
       </c>
       <c r="R18" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O18,N18),Q18)</f>
-        <v>FixedIborSwapCurveNode@249</v>
+        <v>FixedIborSwapCurveNode@7</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.45">
@@ -1208,11 +1220,11 @@
       </c>
       <c r="E19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B19&amp;"."&amp;C19)</f>
-        <v>QuoteId@609</v>
+        <v>QuoteId@15</v>
       </c>
       <c r="F19" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C19,B19),E19)</f>
-        <v>FixedOvernightSwapCurveNode@244</v>
+        <v>FixedOvernightSwapCurveNode@4</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>75</v>
@@ -1225,14 +1237,14 @@
       </c>
       <c r="K19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H19&amp;"."&amp;I19)</f>
-        <v>QuoteId@599</v>
+        <v>QuoteId@19</v>
       </c>
       <c r="L19" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I19,H19),K19)</f>
-        <v>FixedIborSwapCurveNode@258</v>
+        <v>FixedIborSwapCurveNode@8</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="O19" s="12" t="s">
         <v>41</v>
@@ -1242,11 +1254,11 @@
       </c>
       <c r="Q19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N19&amp;"."&amp;O19)</f>
-        <v>QuoteId@583</v>
+        <v>QuoteId@17</v>
       </c>
       <c r="R19" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O19,N19),Q19)</f>
-        <v>FixedIborSwapCurveNode@248</v>
+        <v>FixedIborSwapCurveNode@5</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.45">
@@ -1261,11 +1273,11 @@
       </c>
       <c r="E20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B20&amp;"."&amp;C20)</f>
-        <v>QuoteId@607</v>
+        <v>QuoteId@22</v>
       </c>
       <c r="F20" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C20,B20),E20)</f>
-        <v>FixedOvernightSwapCurveNode@249</v>
+        <v>FixedOvernightSwapCurveNode@6</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>75</v>
@@ -1278,14 +1290,14 @@
       </c>
       <c r="K20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H20&amp;"."&amp;I20)</f>
-        <v>QuoteId@597</v>
+        <v>QuoteId@18</v>
       </c>
       <c r="L20" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I20,H20),K20)</f>
-        <v>FixedIborSwapCurveNode@260</v>
+        <v>FixedIborSwapCurveNode@6</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="O20" s="12" t="s">
         <v>42</v>
@@ -1295,11 +1307,11 @@
       </c>
       <c r="Q20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N20&amp;"."&amp;O20)</f>
-        <v>QuoteId@588</v>
+        <v>QuoteId@23</v>
       </c>
       <c r="R20" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O20,N20),Q20)</f>
-        <v>FixedIborSwapCurveNode@251</v>
+        <v>FixedIborSwapCurveNode@10</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.45">
@@ -1314,11 +1326,11 @@
       </c>
       <c r="E21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B21&amp;"."&amp;C21)</f>
-        <v>QuoteId@610</v>
+        <v>QuoteId@20</v>
       </c>
       <c r="F21" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C21,B21),E21)</f>
-        <v>FixedOvernightSwapCurveNode@245</v>
+        <v>FixedOvernightSwapCurveNode@9</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>75</v>
@@ -1331,14 +1343,14 @@
       </c>
       <c r="K21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H21&amp;"."&amp;I21)</f>
-        <v>QuoteId@598</v>
+        <v>QuoteId@25</v>
       </c>
       <c r="L21" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I21,H21),K21)</f>
-        <v>FixedIborSwapCurveNode@257</v>
+        <v>FixedIborSwapCurveNode@11</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="O21" s="12" t="s">
         <v>43</v>
@@ -1348,11 +1360,11 @@
       </c>
       <c r="Q21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N21&amp;"."&amp;O21)</f>
-        <v>QuoteId@582</v>
+        <v>QuoteId@21</v>
       </c>
       <c r="R21" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O21,N21),Q21)</f>
-        <v>FixedIborSwapCurveNode@246</v>
+        <v>FixedIborSwapCurveNode@9</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.45">
@@ -1367,11 +1379,11 @@
       </c>
       <c r="E22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B22&amp;"."&amp;C22)</f>
-        <v>QuoteId@608</v>
+        <v>QuoteId@26</v>
       </c>
       <c r="F22" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C22,B22),E22)</f>
-        <v>FixedOvernightSwapCurveNode@243</v>
+        <v>FixedOvernightSwapCurveNode@7</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>75</v>
@@ -1384,14 +1396,14 @@
       </c>
       <c r="K22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H22&amp;"."&amp;I22)</f>
-        <v>QuoteId@600</v>
+        <v>QuoteId@31</v>
       </c>
       <c r="L22" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I22,H22),K22)</f>
-        <v>FixedIborSwapCurveNode@261</v>
+        <v>FixedIborSwapCurveNode@15</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="O22" s="12" t="s">
         <v>44</v>
@@ -1401,11 +1413,11 @@
       </c>
       <c r="Q22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N22&amp;"."&amp;O22)</f>
-        <v>QuoteId@581</v>
+        <v>QuoteId@27</v>
       </c>
       <c r="R22" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O22,N22),Q22)</f>
-        <v>FixedIborSwapCurveNode@245</v>
+        <v>FixedIborSwapCurveNode@12</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.45">
@@ -1420,11 +1432,11 @@
       </c>
       <c r="E23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B23&amp;"."&amp;C23)</f>
-        <v>QuoteId@612</v>
+        <v>QuoteId@24</v>
       </c>
       <c r="F23" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C23,B23),E23)</f>
-        <v>FixedOvernightSwapCurveNode@248</v>
+        <v>FixedOvernightSwapCurveNode@8</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>75</v>
@@ -1437,14 +1449,14 @@
       </c>
       <c r="K23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H23&amp;"."&amp;I23)</f>
-        <v>QuoteId@595</v>
+        <v>QuoteId@28</v>
       </c>
       <c r="L23" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I23,H23),K23)</f>
-        <v>FixedIborSwapCurveNode@259</v>
+        <v>FixedIborSwapCurveNode@13</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="O23" s="12" t="s">
         <v>45</v>
@@ -1454,11 +1466,11 @@
       </c>
       <c r="Q23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N23&amp;"."&amp;O23)</f>
-        <v>QuoteId@580</v>
+        <v>QuoteId@34</v>
       </c>
       <c r="R23" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O23,N23),Q23)</f>
-        <v>FixedIborSwapCurveNode@247</v>
+        <v>FixedIborSwapCurveNode@17</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.45">
@@ -1473,11 +1485,11 @@
       </c>
       <c r="E24" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B24&amp;"."&amp;C24)</f>
-        <v>QuoteId@615</v>
+        <v>QuoteId@30</v>
       </c>
       <c r="F24" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C24,B24),E24)</f>
-        <v>FixedOvernightSwapCurveNode@251</v>
+        <v>FixedOvernightSwapCurveNode@10</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>75</v>
@@ -1490,14 +1502,14 @@
       </c>
       <c r="K24" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H24&amp;"."&amp;I24)</f>
-        <v>QuoteId@594</v>
+        <v>QuoteId@29</v>
       </c>
       <c r="L24" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I24,H24),K24)</f>
-        <v>FixedIborSwapCurveNode@255</v>
+        <v>FixedIborSwapCurveNode@14</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="O24" s="12" t="s">
         <v>46</v>
@@ -1507,11 +1519,11 @@
       </c>
       <c r="Q24" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N24&amp;"."&amp;O24)</f>
-        <v>QuoteId@578</v>
+        <v>QuoteId@32</v>
       </c>
       <c r="R24" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O24,N24),Q24)</f>
-        <v>FixedIborSwapCurveNode@252</v>
+        <v>FixedIborSwapCurveNode@20</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.45">
@@ -1526,11 +1538,11 @@
       </c>
       <c r="E25" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B25&amp;"."&amp;C25)</f>
-        <v>QuoteId@613</v>
+        <v>QuoteId@37</v>
       </c>
       <c r="F25" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C25,B25),E25)</f>
-        <v>FixedOvernightSwapCurveNode@247</v>
+        <v>FixedOvernightSwapCurveNode@11</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>75</v>
@@ -1543,14 +1555,14 @@
       </c>
       <c r="K25" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H25&amp;"."&amp;I25)</f>
-        <v>QuoteId@596</v>
+        <v>QuoteId@33</v>
       </c>
       <c r="L25" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I25,H25),K25)</f>
-        <v>FixedIborSwapCurveNode@256</v>
+        <v>FixedIborSwapCurveNode@16</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="O25" s="12" t="s">
         <v>47</v>
@@ -1560,11 +1572,11 @@
       </c>
       <c r="Q25" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N25&amp;"."&amp;O25)</f>
-        <v>QuoteId@579</v>
+        <v>QuoteId@35</v>
       </c>
       <c r="R25" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O25,N25),Q25)</f>
-        <v>FixedIborSwapCurveNode@244</v>
+        <v>FixedIborSwapCurveNode@18</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.45">
@@ -1579,11 +1591,11 @@
       </c>
       <c r="E26" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B26&amp;"."&amp;C26)</f>
-        <v>QuoteId@611</v>
+        <v>QuoteId@39</v>
       </c>
       <c r="F26" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C26,B26),E26)</f>
-        <v>FixedOvernightSwapCurveNode@246</v>
+        <v>FixedOvernightSwapCurveNode@13</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>75</v>
@@ -1596,11 +1608,11 @@
       </c>
       <c r="K26" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H26&amp;"."&amp;I26)</f>
-        <v>QuoteId@602</v>
+        <v>QuoteId@38</v>
       </c>
       <c r="L26" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I26,H26),K26)</f>
-        <v>FixedIborSwapCurveNode@262</v>
+        <v>FixedIborSwapCurveNode@19</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.45">
@@ -1615,25 +1627,25 @@
       </c>
       <c r="E27" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B27&amp;"."&amp;C27)</f>
-        <v>QuoteId@614</v>
+        <v>QuoteId@36</v>
       </c>
       <c r="F27" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C27,B27),E27)</f>
-        <v>FixedOvernightSwapCurveNode@250</v>
+        <v>FixedOvernightSwapCurveNode@12</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B31" s="16" t="str">
         <f>_xll.og.InterpolatedNodalCurveDefinition.build(B32:B38,C32:C38,F14:F27)</f>
-        <v>InterpolatedNodalCurveDefinition@68</v>
+        <v>InterpolatedNodalCurveDefinition@2</v>
       </c>
       <c r="H31" s="16" t="str">
         <f>_xll.og.InterpolatedNodalCurveDefinition.build(H32:H38,I32:I38,L14:L26)</f>
-        <v>InterpolatedNodalCurveDefinition@67</v>
+        <v>InterpolatedNodalCurveDefinition@3</v>
       </c>
       <c r="N31" s="16" t="str">
         <f>_xll.og.InterpolatedNodalCurveDefinition.build(N32:N38,O32:O38,R14:R25)</f>
-        <v>InterpolatedNodalCurveDefinition@66</v>
+        <v>InterpolatedNodalCurveDefinition@1</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.45">
@@ -1653,7 +1665,7 @@
         <v>48</v>
       </c>
       <c r="O32" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.45">
@@ -1779,15 +1791,15 @@
     <row r="40" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B40" s="16" t="str">
         <f>_xll.og.CurveGroupEntry.of(C41,C42,C43)</f>
-        <v>CurveGroupEntry@43</v>
+        <v>CurveGroupEntry@1</v>
       </c>
       <c r="H40" s="16" t="str">
         <f>_xll.og.CurveGroupEntry.of(I41,I42,I43)</f>
-        <v>CurveGroupEntry@42</v>
+        <v>CurveGroupEntry@3</v>
       </c>
       <c r="N40" s="16" t="str">
         <f>_xll.og.CurveGroupEntry.of(O41,O42,O43)</f>
-        <v>CurveGroupEntry@41</v>
+        <v>CurveGroupEntry@2</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.45">
@@ -1807,7 +1819,7 @@
         <v>48</v>
       </c>
       <c r="O41" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.45">
@@ -1836,7 +1848,7 @@
       </c>
       <c r="C43" s="12" t="str">
         <f>_xll.og.OvernightIndex.of(D43)</f>
-        <v>ImmutableOvernightIndex@14</v>
+        <v>ImmutableOvernightIndex@1</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>62</v>
@@ -1846,7 +1858,7 @@
       </c>
       <c r="I43" s="12" t="str">
         <f>_xll.og.IborIndex.of(J43)</f>
-        <v>ImmutableIborIndex@28</v>
+        <v>ImmutableIborIndex@2</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>71</v>
@@ -1856,10 +1868,10 @@
       </c>
       <c r="O43" s="12" t="str">
         <f>_xll.og.IborIndex.of(P43)</f>
-        <v>ImmutableIborIndex@27</v>
+        <v>ImmutableIborIndex@1</v>
       </c>
       <c r="P43" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1869,7 +1881,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J28"/>
+  <dimension ref="B2:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
@@ -1884,41 +1896,96 @@
     <col min="8" max="8" width="24.3984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.59765625" customWidth="1"/>
+    <col min="15" max="15" width="21.9296875" customWidth="1"/>
+    <col min="16" max="16" width="22.59765625" customWidth="1"/>
+    <col min="17" max="17" width="18.796875" customWidth="1"/>
+    <col min="18" max="18" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28" customWidth="1"/>
+    <col min="20" max="20" width="24" customWidth="1"/>
+    <col min="21" max="21" width="18.19921875" customWidth="1"/>
+    <col min="22" max="22" width="15" customWidth="1"/>
+    <col min="23" max="23" width="11.86328125" customWidth="1"/>
+    <col min="24" max="24" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B2" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="8" t="str">
         <f>_xll.og.ReferenceData.standard()</f>
-        <v>ImmutableReferenceData@24</v>
+        <v>ImmutableReferenceData@1</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>69</v>
       </c>
       <c r="F2" s="20" t="str">
         <f>_xll.og.DiscountingSwapProductPricer.DEFAULT()</f>
-        <v>DiscountingSwapProductPricer@10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+        <v>DiscountingSwapProductPricer@1</v>
+      </c>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q2" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B3" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="str">
         <f>_xll.og.Swap.resolve(C5,C2)</f>
-        <v>ResolvedSwap@10</v>
+        <v>ResolvedSwap@1</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F3" s="20" t="str">
         <f>_xll.og.DiscountingSwapProductPricer.presentValueMultiCurrency(F2,C3,'Market Data'!B2)</f>
-        <v>MultiCurrencyAmount@5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+        <v>MultiCurrencyAmount@1</v>
+      </c>
+      <c r="L3" s="3" t="str">
+        <f t="array" ref="L3:L18">_xll.og.List.explode(F5)</f>
+        <v>IborRateSensitivity@1</v>
+      </c>
+      <c r="M3" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L3,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N3" s="20" t="str">
+        <f>_xll.og.Bean.property($L3,N$2)</f>
+        <v/>
+      </c>
+      <c r="O3" s="23" t="str">
+        <f>_xll.og.Bean.property($L3,O$2)</f>
+        <v>EUR-EURIBOR-3M</v>
+      </c>
+      <c r="P3" s="20">
+        <f>_xll.og.Bean.property($L3,P$2)</f>
+        <v>0.25555555555555554</v>
+      </c>
+      <c r="Q3" s="24">
+        <f>_xll.og.Bean.property($L3,Q$2)</f>
+        <v>2556450.1789434357</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
       <c r="E4" s="19" t="s">
         <v>78</v>
       </c>
@@ -1926,51 +1993,198 @@
         <f>_xll.og.CurrencyAmount.getAmount(_xll.og.MultiCurrencyAmount.getAmountOrZero(F3,"EUR"))</f>
         <v>-272455.95127698663</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="L4" s="3" t="str">
+        <v>IborRateSensitivity@2</v>
+      </c>
+      <c r="M4" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L4,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N4" s="20" t="str">
+        <f>_xll.og.Bean.property($L4,N$2)</f>
+        <v/>
+      </c>
+      <c r="O4" s="23" t="str">
+        <f>_xll.og.Bean.property($L4,O$2)</f>
+        <v>EUR-EURIBOR-3M</v>
+      </c>
+      <c r="P4" s="20">
+        <f>_xll.og.Bean.property($L4,P$2)</f>
+        <v>0.25555555555555554</v>
+      </c>
+      <c r="Q4" s="24">
+        <f>_xll.og.Bean.property($L4,Q$2)</f>
+        <v>2557326.0710469773</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B5" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="8" t="str">
         <f>_xll.og.Swap.of(C6:C7)</f>
-        <v>Swap@10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+        <v>Swap@1</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="21" t="str">
+        <f>_xll.og.PointSensitivities.getSensitivities(_xll.og.PointSensitivities.normalized(_xll.og.PointSensitivityBuilder.build(_xll.og.DiscountingSwapProductPricer.presentValueSensitivity(F2,C3,'Market Data'!B2))))</f>
+        <v>RegularImmutableList@1</v>
+      </c>
+      <c r="L5" s="3" t="str">
+        <v>IborRateSensitivity@3</v>
+      </c>
+      <c r="M5" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L5,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N5" s="20" t="str">
+        <f>_xll.og.Bean.property($L5,N$2)</f>
+        <v/>
+      </c>
+      <c r="O5" s="23" t="str">
+        <f>_xll.og.Bean.property($L5,O$2)</f>
+        <v>EUR-EURIBOR-3M</v>
+      </c>
+      <c r="P5" s="20">
+        <f>_xll.og.Bean.property($L5,P$2)</f>
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="Q5" s="24">
+        <f>_xll.og.Bean.property($L5,Q$2)</f>
+        <v>2531429.3182908599</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>C9</f>
-        <v>RateCalculationSwapLeg@20</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+        <v>RateCalculationSwapLeg@2</v>
+      </c>
+      <c r="L6" s="3" t="str">
+        <v>IborRateSensitivity@4</v>
+      </c>
+      <c r="M6" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L6,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N6" s="20" t="str">
+        <f>_xll.og.Bean.property($L6,N$2)</f>
+        <v/>
+      </c>
+      <c r="O6" s="23" t="str">
+        <f>_xll.og.Bean.property($L6,O$2)</f>
+        <v>EUR-EURIBOR-3M</v>
+      </c>
+      <c r="P6" s="20">
+        <f>_xll.og.Bean.property($L6,P$2)</f>
+        <v>0.25</v>
+      </c>
+      <c r="Q6" s="24">
+        <f>_xll.og.Bean.property($L6,Q$2)</f>
+        <v>2504777.6951774531</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>H9</f>
-        <v>RateCalculationSwapLeg@19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+        <v>RateCalculationSwapLeg@1</v>
+      </c>
+      <c r="L7" s="3" t="str">
+        <v>IborRateSensitivity@5</v>
+      </c>
+      <c r="M7" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L7,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N7" s="20" t="str">
+        <f>_xll.og.Bean.property($L7,N$2)</f>
+        <v/>
+      </c>
+      <c r="O7" s="23" t="str">
+        <f>_xll.og.Bean.property($L7,O$2)</f>
+        <v>EUR-EURIBOR-3M</v>
+      </c>
+      <c r="P7" s="20">
+        <f>_xll.og.Bean.property($L7,P$2)</f>
+        <v>0.25555555555555554</v>
+      </c>
+      <c r="Q7" s="24">
+        <f>_xll.og.Bean.property($L7,Q$2)</f>
+        <v>2561913.0308725024</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="L8" s="3" t="str">
+        <v>IborRateSensitivity@6</v>
+      </c>
+      <c r="M8" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L8,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N8" s="20" t="str">
+        <f>_xll.og.Bean.property($L8,N$2)</f>
+        <v/>
+      </c>
+      <c r="O8" s="23" t="str">
+        <f>_xll.og.Bean.property($L8,O$2)</f>
+        <v>EUR-EURIBOR-3M</v>
+      </c>
+      <c r="P8" s="20">
+        <f>_xll.og.Bean.property($L8,P$2)</f>
+        <v>0.26111111111111113</v>
+      </c>
+      <c r="Q8" s="24">
+        <f>_xll.og.Bean.property($L8,Q$2)</f>
+        <v>2619250.9833476138</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="8" t="str">
         <f>_xll.og.RateCalculationSwapLeg.build(B10:B14,C10:C14)</f>
-        <v>RateCalculationSwapLeg@20</v>
+        <v>RateCalculationSwapLeg@2</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="8" t="str">
         <f>_xll.og.RateCalculationSwapLeg.build(G10:G14,H10:H14)</f>
-        <v>RateCalculationSwapLeg@19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+        <v>RateCalculationSwapLeg@1</v>
+      </c>
+      <c r="L9" s="3" t="str">
+        <v>IborRateSensitivity@7</v>
+      </c>
+      <c r="M9" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L9,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N9" s="20" t="str">
+        <f>_xll.og.Bean.property($L9,N$2)</f>
+        <v/>
+      </c>
+      <c r="O9" s="23" t="str">
+        <f>_xll.og.Bean.property($L9,O$2)</f>
+        <v>EUR-EURIBOR-3M</v>
+      </c>
+      <c r="P9" s="20">
+        <f>_xll.og.Bean.property($L9,P$2)</f>
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="Q9" s="24">
+        <f>_xll.og.Bean.property($L9,Q$2)</f>
+        <v>2537297.6014800463</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
@@ -1983,62 +2197,154 @@
       <c r="H10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="L10" s="3" t="str">
+        <v>IborRateSensitivity@8</v>
+      </c>
+      <c r="M10" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L10,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N10" s="20" t="str">
+        <f>_xll.og.Bean.property($L10,N$2)</f>
+        <v/>
+      </c>
+      <c r="O10" s="23" t="str">
+        <f>_xll.og.Bean.property($L10,O$2)</f>
+        <v>EUR-EURIBOR-3M</v>
+      </c>
+      <c r="P10" s="20">
+        <f>_xll.og.Bean.property($L10,P$2)</f>
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="Q10" s="24">
+        <f>_xll.og.Bean.property($L10,Q$2)</f>
+        <v>2455273.4145536497</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>C16</f>
-        <v>PeriodicSchedule@20</v>
+        <v>PeriodicSchedule@2</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H11" s="1" t="str">
         <f>H16</f>
-        <v>PeriodicSchedule@19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
+        <v>PeriodicSchedule@1</v>
+      </c>
+      <c r="L11" s="3" t="str">
+        <v>ZeroRateSensitivity@1</v>
+      </c>
+      <c r="M11" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L11,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N11" s="25">
+        <f>_xll.og.Bean.property($L11,N$2)</f>
+        <v>0.25753424657534246</v>
+      </c>
+      <c r="O11" s="23" t="str">
+        <f>_xll.og.Bean.property($L11,O$2)</f>
+        <v/>
+      </c>
+      <c r="P11" s="20" t="str">
+        <f>_xll.og.Bean.property($L11,P$2)</f>
+        <v/>
+      </c>
+      <c r="Q11" s="24">
+        <f>_xll.og.Bean.property($L11,Q$2)</f>
+        <v>7933.4003224362186</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="str">
         <f>C22</f>
-        <v>PaymentSchedule@20</v>
+        <v>PaymentSchedule@1</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="1" t="str">
         <f>H22</f>
-        <v>PaymentSchedule@19</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
+        <v>PaymentSchedule@2</v>
+      </c>
+      <c r="L12" s="3" t="str">
+        <v>ZeroRateSensitivity@2</v>
+      </c>
+      <c r="M12" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L12,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N12" s="20">
+        <f>_xll.og.Bean.property($L12,N$2)</f>
+        <v>0.50958904109589043</v>
+      </c>
+      <c r="O12" s="23" t="str">
+        <f>_xll.og.Bean.property($L12,O$2)</f>
+        <v/>
+      </c>
+      <c r="P12" s="20" t="str">
+        <f>_xll.og.Bean.property($L12,P$2)</f>
+        <v/>
+      </c>
+      <c r="Q12" s="24">
+        <f>_xll.og.Bean.property($L12,Q$2)</f>
+        <v>17071.727958181815</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>_xll.og.NotionalSchedule.build(B27:B28,C27:C28)</f>
-        <v>NotionalSchedule@30</v>
+        <v>NotionalSchedule@1</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="1" t="str">
         <f>H26</f>
-        <v>NotionalSchedule@28</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
+        <v>NotionalSchedule@2</v>
+      </c>
+      <c r="L13" s="3" t="str">
+        <v>ZeroRateSensitivity@3</v>
+      </c>
+      <c r="M13" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L13,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N13" s="20">
+        <f>_xll.og.Bean.property($L13,N$2)</f>
+        <v>0.75890410958904109</v>
+      </c>
+      <c r="O13" s="23" t="str">
+        <f>_xll.og.Bean.property($L13,O$2)</f>
+        <v/>
+      </c>
+      <c r="P13" s="20" t="str">
+        <f>_xll.og.Bean.property($L13,P$2)</f>
+        <v/>
+      </c>
+      <c r="Q13" s="24">
+        <f>_xll.og.Bean.property($L13,Q$2)</f>
+        <v>25166.568677485251</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>_xll.og.FixedRateCalculation.of(D14,E14)</f>
-        <v>FixedRateCalculation@10</v>
+        <v>FixedRateCalculation@1</v>
       </c>
       <c r="D14" s="7">
         <v>0.01</v>
@@ -2051,29 +2357,100 @@
       </c>
       <c r="H14" s="1" t="str">
         <f>_xll.og.IborRateCalculation.of(I14)</f>
-        <v>IborRateCalculation@10</v>
+        <v>IborRateCalculation@1</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="L14" s="3" t="str">
+        <v>ZeroRateSensitivity@4</v>
+      </c>
+      <c r="M14" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L14,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N14" s="20">
+        <f>_xll.og.Bean.property($L14,N$2)</f>
+        <v>1.0054794520547945</v>
+      </c>
+      <c r="O14" s="23" t="str">
+        <f>_xll.og.Bean.property($L14,O$2)</f>
+        <v/>
+      </c>
+      <c r="P14" s="20" t="str">
+        <f>_xll.og.Bean.property($L14,P$2)</f>
+        <v/>
+      </c>
+      <c r="Q14" s="24">
+        <f>_xll.og.Bean.property($L14,Q$2)</f>
+        <v>35787.13660480408</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="L15" s="3" t="str">
+        <v>ZeroRateSensitivity@5</v>
+      </c>
+      <c r="M15" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L15,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N15" s="20">
+        <f>_xll.og.Bean.property($L15,N$2)</f>
+        <v>1.2575342465753425</v>
+      </c>
+      <c r="O15" s="23" t="str">
+        <f>_xll.og.Bean.property($L15,O$2)</f>
+        <v/>
+      </c>
+      <c r="P15" s="20" t="str">
+        <f>_xll.og.Bean.property($L15,P$2)</f>
+        <v/>
+      </c>
+      <c r="Q15" s="24">
+        <f>_xll.og.Bean.property($L15,Q$2)</f>
+        <v>43439.604779939771</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="8" t="str">
         <f>_xll.og.PeriodicSchedule.build(B17:B20,C17:C20)</f>
-        <v>PeriodicSchedule@20</v>
+        <v>PeriodicSchedule@2</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="8" t="str">
         <f>_xll.og.PeriodicSchedule.build(G17:G20,H17:H20)</f>
-        <v>PeriodicSchedule@19</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
+        <v>PeriodicSchedule@1</v>
+      </c>
+      <c r="L16" s="3" t="str">
+        <v>ZeroRateSensitivity@6</v>
+      </c>
+      <c r="M16" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L16,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N16" s="20">
+        <f>_xll.og.Bean.property($L16,N$2)</f>
+        <v>1.515068493150685</v>
+      </c>
+      <c r="O16" s="23" t="str">
+        <f>_xll.og.Bean.property($L16,O$2)</f>
+        <v/>
+      </c>
+      <c r="P16" s="20" t="str">
+        <f>_xll.og.Bean.property($L16,P$2)</f>
+        <v/>
+      </c>
+      <c r="Q16" s="24">
+        <f>_xll.og.Bean.property($L16,Q$2)</f>
+        <v>54118.288769099832</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
@@ -2086,8 +2463,31 @@
       <c r="H17" s="5">
         <v>42431</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="L17" s="3" t="str">
+        <v>ZeroRateSensitivity@7</v>
+      </c>
+      <c r="M17" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L17,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N17" s="20">
+        <f>_xll.og.Bean.property($L17,N$2)</f>
+        <v>1.7643835616438357</v>
+      </c>
+      <c r="O17" s="23" t="str">
+        <f>_xll.og.Bean.property($L17,O$2)</f>
+        <v/>
+      </c>
+      <c r="P17" s="20" t="str">
+        <f>_xll.og.Bean.property($L17,P$2)</f>
+        <v/>
+      </c>
+      <c r="Q17" s="24">
+        <f>_xll.og.Bean.property($L17,Q$2)</f>
+        <v>61738.114744073675</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
@@ -2100,8 +2500,31 @@
       <c r="H18" s="5">
         <v>43161</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="L18" s="3" t="str">
+        <v>ZeroRateSensitivity@8</v>
+      </c>
+      <c r="M18" s="20" t="str">
+        <f>_xll.og.Currency.toString(_xll.og.Bean.property($L18,M$2))</f>
+        <v>EUR</v>
+      </c>
+      <c r="N18" s="20">
+        <f>_xll.og.Bean.property($L18,N$2)</f>
+        <v>2.0054794520547947</v>
+      </c>
+      <c r="O18" s="23" t="str">
+        <f>_xll.og.Bean.property($L18,O$2)</f>
+        <v/>
+      </c>
+      <c r="P18" s="20" t="str">
+        <f>_xll.og.Bean.property($L18,P$2)</f>
+        <v/>
+      </c>
+      <c r="Q18" s="24">
+        <f>_xll.og.Bean.property($L18,Q$2)</f>
+        <v>68469.259415752371</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
@@ -2115,13 +2538,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="1" t="str">
         <f>_xll.og.BusinessDayAdjustment.of(D20,E20)</f>
-        <v>BusinessDayAdjustment@20</v>
+        <v>BusinessDayAdjustment@1</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>7</v>
@@ -2134,7 +2557,7 @@
       </c>
       <c r="H20" s="1" t="str">
         <f>_xll.og.BusinessDayAdjustment.of(I20,J20)</f>
-        <v>BusinessDayAdjustment@19</v>
+        <v>BusinessDayAdjustment@2</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>7</v>
@@ -2143,23 +2566,25 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="8" t="str">
         <f>_xll.og.PaymentSchedule.build(B23:B24,C23:C24)</f>
-        <v>PaymentSchedule@20</v>
+        <v>PaymentSchedule@1</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H22" s="8" t="str">
         <f>_xll.og.PaymentSchedule.build(G23:G24,H23:H24)</f>
-        <v>PaymentSchedule@19</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.45">
+        <v>PaymentSchedule@2</v>
+      </c>
+      <c r="O22" s="22"/>
+      <c r="Q22" s="6"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
@@ -2172,8 +2597,10 @@
       <c r="H23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="O23" s="22"/>
+      <c r="Q23" s="6"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
         <v>9</v>
       </c>
@@ -2186,24 +2613,32 @@
       <c r="H24" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="O24" s="22"/>
+      <c r="Q24" s="6"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="O25" s="22"/>
+      <c r="Q25" s="6"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B26" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="8" t="str">
         <f>_xll.og.NotionalSchedule.build(B27:B28,C27:C28)</f>
-        <v>NotionalSchedule@29</v>
+        <v>NotionalSchedule@3</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H26" s="8" t="str">
         <f>_xll.og.NotionalSchedule.build(G27:G28,H27:H28)</f>
-        <v>NotionalSchedule@28</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.45">
+        <v>NotionalSchedule@2</v>
+      </c>
+      <c r="O26" s="22"/>
+      <c r="Q26" s="6"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B27" s="2" t="s">
         <v>12</v>
       </c>
@@ -2216,8 +2651,10 @@
       <c r="H27" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="O27" s="22"/>
+      <c r="Q27" s="6"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
         <v>13</v>
       </c>
@@ -2231,8 +2668,17 @@
       <c r="H28" s="14">
         <v>10000000</v>
       </c>
+      <c r="O28" s="22"/>
+      <c r="Q28" s="6"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="O29" s="22"/>
+      <c r="Q29" s="6"/>
     </row>
   </sheetData>
+  <sortState ref="Y6:Z29">
+    <sortCondition ref="Y6:Y29"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update to Strata 2.0.0
</commit_message>
<xml_diff>
--- a/examples/swap-pricer.xlsx
+++ b/examples/swap-pricer.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\strata-excel\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E3A67379-4C00-483A-ADC6-FE37DCAED699}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="3953" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="3960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Market Data" sheetId="2" r:id="rId1"/>
     <sheet name="Swap" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -294,7 +295,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
@@ -778,38 +779,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R43"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" customWidth="1"/>
-    <col min="2" max="5" width="33.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.9296875" customWidth="1"/>
-    <col min="8" max="8" width="33.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.1328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="str">
-        <f>_xll.og.CurveCalibrator.calibrate(_xll.og.CurveCalibrator.standard(),B8,C4,C6)</f>
-        <v>ImmutableRatesProvider@1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.45">
+        <f>_xll.og.RatesCurveCalibrator.calibrate(_xll.og.RatesCurveCalibrator.standard(),B8,C4,C6)</f>
+        <v>ImmutableRatesProvider@2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>67</v>
       </c>
@@ -817,48 +816,48 @@
         <v>42429</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="17" t="str">
         <f>_xll.og.MarketData.combinedWith(_xll.og.MarketData.combinedWith(C5,D5),E5)</f>
-        <v>ImmutableMarketData@5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+        <v>ImmutableMarketData@10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C5" s="12" t="str">
         <f>_xll.og.MarketData.of(C3,E14:E27,D14:D27)</f>
-        <v>ImmutableMarketData@1</v>
+        <v>ImmutableMarketData@6</v>
       </c>
       <c r="D5" s="12" t="str">
         <f>_xll.og.MarketData.of(C3,K14:K26,J14:J26)</f>
-        <v>ImmutableMarketData@3</v>
+        <v>ImmutableMarketData@8</v>
       </c>
       <c r="E5" s="12" t="str">
         <f>_xll.og.MarketData.of(C3,Q14:Q25,P14:P25)</f>
-        <v>ImmutableMarketData@2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.45">
+        <v>ImmutableMarketData@7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="12" t="str">
         <f>_xll.og.ReferenceData.standard()</f>
-        <v>ImmutableReferenceData@2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.45">
+        <v>ImmutableReferenceData@4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="str">
-        <f>_xll.og.CurveGroupDefinition.of(C9,C10:E10,C11:E11)</f>
-        <v>CurveGroupDefinition@1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.45">
+        <f>_xll.og.RatesCurveGroupDefinition.of(C9,C10:E10,C11:E11)</f>
+        <v>RatesCurveGroupDefinition@2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>48</v>
       </c>
@@ -866,41 +865,41 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="12" t="str">
         <f>B40</f>
-        <v>CurveGroupEntry@1</v>
+        <v>RatesCurveGroupEntry@4</v>
       </c>
       <c r="D10" s="12" t="str">
         <f>H40</f>
-        <v>CurveGroupEntry@3</v>
+        <v>RatesCurveGroupEntry@5</v>
       </c>
       <c r="E10" s="12" t="str">
         <f>N40</f>
-        <v>CurveGroupEntry@2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.45">
+        <v>RatesCurveGroupEntry@6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C11" s="12" t="str">
         <f>B31</f>
-        <v>InterpolatedNodalCurveDefinition@2</v>
+        <v>InterpolatedNodalCurveDefinition@4</v>
       </c>
       <c r="D11" s="12" t="str">
         <f>H31</f>
-        <v>InterpolatedNodalCurveDefinition@3</v>
+        <v>InterpolatedNodalCurveDefinition@5</v>
       </c>
       <c r="E11" s="12" t="str">
         <f>N31</f>
-        <v>InterpolatedNodalCurveDefinition@1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.45">
+        <v>InterpolatedNodalCurveDefinition@6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
@@ -947,7 +946,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
         <v>29</v>
       </c>
@@ -959,11 +958,11 @@
       </c>
       <c r="E14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B14&amp;"."&amp;C14)</f>
-        <v>QuoteId@7</v>
+        <v>QuoteId@41</v>
       </c>
       <c r="F14" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C14,B14),E14)</f>
-        <v>FixedOvernightSwapCurveNode@14</v>
+        <v>FixedOvernightSwapCurveNode@28</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>71</v>
@@ -974,11 +973,11 @@
       </c>
       <c r="K14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H14&amp;"."&amp;I14)</f>
-        <v>QuoteId@2</v>
+        <v>QuoteId@40</v>
       </c>
       <c r="L14" s="13" t="str">
         <f>_xll.og.IborFixingDepositCurveNode.ofRate( _xll.og.IborFixingDepositTemplate.of(H14),K14)</f>
-        <v>IborFixingDepositCurveNode@2</v>
+        <v>IborFixingDepositCurveNode@3</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>79</v>
@@ -989,14 +988,14 @@
       </c>
       <c r="Q14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N14&amp;"."&amp;O14)</f>
-        <v>QuoteId@1</v>
+        <v>QuoteId@42</v>
       </c>
       <c r="R14" s="13" t="str">
         <f>_xll.og.IborFixingDepositCurveNode.ofRate( _xll.og.IborFixingDepositTemplate.of(N14),Q14)</f>
-        <v>IborFixingDepositCurveNode@1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.45">
+        <v>IborFixingDepositCurveNode@4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
         <v>29</v>
       </c>
@@ -1008,11 +1007,11 @@
       </c>
       <c r="E15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B15&amp;"."&amp;C15)</f>
-        <v>QuoteId@5</v>
+        <v>QuoteId@49</v>
       </c>
       <c r="F15" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C15,B15),E15)</f>
-        <v>FixedOvernightSwapCurveNode@1</v>
+        <v>FixedOvernightSwapCurveNode@17</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>71</v>
@@ -1025,11 +1024,11 @@
       </c>
       <c r="K15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H15&amp;"."&amp;I15)</f>
-        <v>QuoteId@8</v>
+        <v>QuoteId@43</v>
       </c>
       <c r="L15" s="13" t="str">
         <f>_xll.og.FraCurveNode.ofRate(_xll.og.FraTemplate.ofIndex(I15,H15),K15)</f>
-        <v>FraCurveNode@2</v>
+        <v>FraCurveNode@5</v>
       </c>
       <c r="N15" s="12" t="s">
         <v>79</v>
@@ -1042,14 +1041,14 @@
       </c>
       <c r="Q15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N15&amp;"."&amp;O15)</f>
-        <v>QuoteId@4</v>
+        <v>QuoteId@44</v>
       </c>
       <c r="R15" s="13" t="str">
         <f>_xll.og.FraCurveNode.ofRate(_xll.og.FraTemplate.ofIndex(O15,N15),Q15)</f>
-        <v>FraCurveNode@1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FraCurveNode@4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>29</v>
       </c>
@@ -1061,11 +1060,11 @@
       </c>
       <c r="E16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B16&amp;"."&amp;C16)</f>
-        <v>QuoteId@3</v>
+        <v>QuoteId@45</v>
       </c>
       <c r="F16" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C16,B16),E16)</f>
-        <v>FixedOvernightSwapCurveNode@3</v>
+        <v>FixedOvernightSwapCurveNode@15</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>71</v>
@@ -1078,11 +1077,11 @@
       </c>
       <c r="K16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H16&amp;"."&amp;I16)</f>
-        <v>QuoteId@10</v>
+        <v>QuoteId@52</v>
       </c>
       <c r="L16" s="13" t="str">
         <f>_xll.og.FraCurveNode.ofRate(_xll.og.FraTemplate.ofIndex(I16,H16),K16)</f>
-        <v>FraCurveNode@3</v>
+        <v>FraCurveNode@6</v>
       </c>
       <c r="N16" s="12" t="s">
         <v>80</v>
@@ -1095,14 +1094,14 @@
       </c>
       <c r="Q16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N16&amp;"."&amp;O16)</f>
-        <v>QuoteId@9</v>
+        <v>QuoteId@47</v>
       </c>
       <c r="R16" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O16,N16),Q16)</f>
-        <v>FixedIborSwapCurveNode@4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
         <v>29</v>
       </c>
@@ -1114,11 +1113,11 @@
       </c>
       <c r="E17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B17&amp;"."&amp;C17)</f>
-        <v>QuoteId@6</v>
+        <v>QuoteId@46</v>
       </c>
       <c r="F17" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C17,B17),E17)</f>
-        <v>FixedOvernightSwapCurveNode@2</v>
+        <v>FixedOvernightSwapCurveNode@16</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>75</v>
@@ -1131,11 +1130,11 @@
       </c>
       <c r="K17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H17&amp;"."&amp;I17)</f>
-        <v>QuoteId@12</v>
+        <v>QuoteId@48</v>
       </c>
       <c r="L17" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I17,H17),K17)</f>
-        <v>FixedIborSwapCurveNode@3</v>
+        <v>FixedIborSwapCurveNode@22</v>
       </c>
       <c r="N17" s="12" t="s">
         <v>80</v>
@@ -1148,14 +1147,14 @@
       </c>
       <c r="Q17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N17&amp;"."&amp;O17)</f>
-        <v>QuoteId@13</v>
+        <v>QuoteId@58</v>
       </c>
       <c r="R17" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O17,N17),Q17)</f>
-        <v>FixedIborSwapCurveNode@1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>29</v>
       </c>
@@ -1167,11 +1166,11 @@
       </c>
       <c r="E18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B18&amp;"."&amp;C18)</f>
-        <v>QuoteId@16</v>
+        <v>QuoteId@55</v>
       </c>
       <c r="F18" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C18,B18),E18)</f>
-        <v>FixedOvernightSwapCurveNode@5</v>
+        <v>FixedOvernightSwapCurveNode@19</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>75</v>
@@ -1184,11 +1183,11 @@
       </c>
       <c r="K18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H18&amp;"."&amp;I18)</f>
-        <v>QuoteId@11</v>
+        <v>QuoteId@51</v>
       </c>
       <c r="L18" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I18,H18),K18)</f>
-        <v>FixedIborSwapCurveNode@2</v>
+        <v>FixedIborSwapCurveNode@24</v>
       </c>
       <c r="N18" s="12" t="s">
         <v>80</v>
@@ -1201,14 +1200,14 @@
       </c>
       <c r="Q18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N18&amp;"."&amp;O18)</f>
-        <v>QuoteId@14</v>
+        <v>QuoteId@50</v>
       </c>
       <c r="R18" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O18,N18),Q18)</f>
-        <v>FixedIborSwapCurveNode@7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>29</v>
       </c>
@@ -1220,11 +1219,11 @@
       </c>
       <c r="E19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B19&amp;"."&amp;C19)</f>
-        <v>QuoteId@15</v>
+        <v>QuoteId@62</v>
       </c>
       <c r="F19" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C19,B19),E19)</f>
-        <v>FixedOvernightSwapCurveNode@4</v>
+        <v>FixedOvernightSwapCurveNode@23</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>75</v>
@@ -1237,11 +1236,11 @@
       </c>
       <c r="K19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H19&amp;"."&amp;I19)</f>
-        <v>QuoteId@19</v>
+        <v>QuoteId@59</v>
       </c>
       <c r="L19" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I19,H19),K19)</f>
-        <v>FixedIborSwapCurveNode@8</v>
+        <v>FixedIborSwapCurveNode@29</v>
       </c>
       <c r="N19" s="12" t="s">
         <v>80</v>
@@ -1254,14 +1253,14 @@
       </c>
       <c r="Q19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N19&amp;"."&amp;O19)</f>
-        <v>QuoteId@17</v>
+        <v>QuoteId@54</v>
       </c>
       <c r="R19" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O19,N19),Q19)</f>
-        <v>FixedIborSwapCurveNode@5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>29</v>
       </c>
@@ -1273,11 +1272,11 @@
       </c>
       <c r="E20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B20&amp;"."&amp;C20)</f>
-        <v>QuoteId@22</v>
+        <v>QuoteId@53</v>
       </c>
       <c r="F20" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C20,B20),E20)</f>
-        <v>FixedOvernightSwapCurveNode@6</v>
+        <v>FixedOvernightSwapCurveNode@18</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>75</v>
@@ -1290,11 +1289,11 @@
       </c>
       <c r="K20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H20&amp;"."&amp;I20)</f>
-        <v>QuoteId@18</v>
+        <v>QuoteId@71</v>
       </c>
       <c r="L20" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I20,H20),K20)</f>
-        <v>FixedIborSwapCurveNode@6</v>
+        <v>FixedIborSwapCurveNode@35</v>
       </c>
       <c r="N20" s="12" t="s">
         <v>80</v>
@@ -1307,14 +1306,14 @@
       </c>
       <c r="Q20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N20&amp;"."&amp;O20)</f>
-        <v>QuoteId@23</v>
+        <v>QuoteId@63</v>
       </c>
       <c r="R20" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O20,N20),Q20)</f>
-        <v>FixedIborSwapCurveNode@10</v>
-      </c>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>29</v>
       </c>
@@ -1326,11 +1325,11 @@
       </c>
       <c r="E21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B21&amp;"."&amp;C21)</f>
-        <v>QuoteId@20</v>
+        <v>QuoteId@57</v>
       </c>
       <c r="F21" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C21,B21),E21)</f>
-        <v>FixedOvernightSwapCurveNode@9</v>
+        <v>FixedOvernightSwapCurveNode@20</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>75</v>
@@ -1343,11 +1342,11 @@
       </c>
       <c r="K21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H21&amp;"."&amp;I21)</f>
-        <v>QuoteId@25</v>
+        <v>QuoteId@56</v>
       </c>
       <c r="L21" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I21,H21),K21)</f>
-        <v>FixedIborSwapCurveNode@11</v>
+        <v>FixedIborSwapCurveNode@26</v>
       </c>
       <c r="N21" s="12" t="s">
         <v>80</v>
@@ -1360,14 +1359,14 @@
       </c>
       <c r="Q21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N21&amp;"."&amp;O21)</f>
-        <v>QuoteId@21</v>
+        <v>QuoteId@73</v>
       </c>
       <c r="R21" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O21,N21),Q21)</f>
-        <v>FixedIborSwapCurveNode@9</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>29</v>
       </c>
@@ -1379,11 +1378,11 @@
       </c>
       <c r="E22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B22&amp;"."&amp;C22)</f>
-        <v>QuoteId@26</v>
+        <v>QuoteId@67</v>
       </c>
       <c r="F22" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C22,B22),E22)</f>
-        <v>FixedOvernightSwapCurveNode@7</v>
+        <v>FixedOvernightSwapCurveNode@22</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>75</v>
@@ -1396,11 +1395,11 @@
       </c>
       <c r="K22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H22&amp;"."&amp;I22)</f>
-        <v>QuoteId@31</v>
+        <v>QuoteId@61</v>
       </c>
       <c r="L22" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I22,H22),K22)</f>
-        <v>FixedIborSwapCurveNode@15</v>
+        <v>FixedIborSwapCurveNode@30</v>
       </c>
       <c r="N22" s="12" t="s">
         <v>80</v>
@@ -1413,14 +1412,14 @@
       </c>
       <c r="Q22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N22&amp;"."&amp;O22)</f>
-        <v>QuoteId@27</v>
+        <v>QuoteId@60</v>
       </c>
       <c r="R22" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O22,N22),Q22)</f>
-        <v>FixedIborSwapCurveNode@12</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@28</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
         <v>29</v>
       </c>
@@ -1432,11 +1431,11 @@
       </c>
       <c r="E23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B23&amp;"."&amp;C23)</f>
-        <v>QuoteId@24</v>
+        <v>QuoteId@76</v>
       </c>
       <c r="F23" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C23,B23),E23)</f>
-        <v>FixedOvernightSwapCurveNode@8</v>
+        <v>FixedOvernightSwapCurveNode@26</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>75</v>
@@ -1449,11 +1448,11 @@
       </c>
       <c r="K23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H23&amp;"."&amp;I23)</f>
-        <v>QuoteId@28</v>
+        <v>QuoteId@70</v>
       </c>
       <c r="L23" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I23,H23),K23)</f>
-        <v>FixedIborSwapCurveNode@13</v>
+        <v>FixedIborSwapCurveNode@34</v>
       </c>
       <c r="N23" s="12" t="s">
         <v>80</v>
@@ -1466,14 +1465,14 @@
       </c>
       <c r="Q23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N23&amp;"."&amp;O23)</f>
-        <v>QuoteId@34</v>
+        <v>QuoteId@65</v>
       </c>
       <c r="R23" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O23,N23),Q23)</f>
-        <v>FixedIborSwapCurveNode@17</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
         <v>29</v>
       </c>
@@ -1485,11 +1484,11 @@
       </c>
       <c r="E24" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B24&amp;"."&amp;C24)</f>
-        <v>QuoteId@30</v>
+        <v>QuoteId@64</v>
       </c>
       <c r="F24" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C24,B24),E24)</f>
-        <v>FixedOvernightSwapCurveNode@10</v>
+        <v>FixedOvernightSwapCurveNode@21</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>75</v>
@@ -1502,11 +1501,11 @@
       </c>
       <c r="K24" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H24&amp;"."&amp;I24)</f>
-        <v>QuoteId@29</v>
+        <v>QuoteId@74</v>
       </c>
       <c r="L24" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I24,H24),K24)</f>
-        <v>FixedIborSwapCurveNode@14</v>
+        <v>FixedIborSwapCurveNode@38</v>
       </c>
       <c r="N24" s="12" t="s">
         <v>80</v>
@@ -1519,14 +1518,14 @@
       </c>
       <c r="Q24" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N24&amp;"."&amp;O24)</f>
-        <v>QuoteId@32</v>
+        <v>QuoteId@72</v>
       </c>
       <c r="R24" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O24,N24),Q24)</f>
-        <v>FixedIborSwapCurveNode@20</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>29</v>
       </c>
@@ -1538,11 +1537,11 @@
       </c>
       <c r="E25" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B25&amp;"."&amp;C25)</f>
-        <v>QuoteId@37</v>
+        <v>QuoteId@68</v>
       </c>
       <c r="F25" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C25,B25),E25)</f>
-        <v>FixedOvernightSwapCurveNode@11</v>
+        <v>FixedOvernightSwapCurveNode@24</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>75</v>
@@ -1555,11 +1554,11 @@
       </c>
       <c r="K25" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H25&amp;"."&amp;I25)</f>
-        <v>QuoteId@33</v>
+        <v>QuoteId@66</v>
       </c>
       <c r="L25" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I25,H25),K25)</f>
-        <v>FixedIborSwapCurveNode@16</v>
+        <v>FixedIborSwapCurveNode@33</v>
       </c>
       <c r="N25" s="12" t="s">
         <v>80</v>
@@ -1572,14 +1571,14 @@
       </c>
       <c r="Q25" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N25&amp;"."&amp;O25)</f>
-        <v>QuoteId@35</v>
+        <v>QuoteId@77</v>
       </c>
       <c r="R25" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O25,N25),Q25)</f>
-        <v>FixedIborSwapCurveNode@18</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>29</v>
       </c>
@@ -1591,11 +1590,11 @@
       </c>
       <c r="E26" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B26&amp;"."&amp;C26)</f>
-        <v>QuoteId@39</v>
+        <v>QuoteId@75</v>
       </c>
       <c r="F26" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C26,B26),E26)</f>
-        <v>FixedOvernightSwapCurveNode@13</v>
+        <v>FixedOvernightSwapCurveNode@27</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>75</v>
@@ -1608,14 +1607,14 @@
       </c>
       <c r="K26" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H26&amp;"."&amp;I26)</f>
-        <v>QuoteId@38</v>
+        <v>QuoteId@78</v>
       </c>
       <c r="L26" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I26,H26),K26)</f>
-        <v>FixedIborSwapCurveNode@19</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FixedIborSwapCurveNode@40</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>29</v>
       </c>
@@ -1627,28 +1626,28 @@
       </c>
       <c r="E27" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B27&amp;"."&amp;C27)</f>
-        <v>QuoteId@36</v>
+        <v>QuoteId@69</v>
       </c>
       <c r="F27" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C27,B27),E27)</f>
-        <v>FixedOvernightSwapCurveNode@12</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.45">
+        <v>FixedOvernightSwapCurveNode@25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="16" t="str">
         <f>_xll.og.InterpolatedNodalCurveDefinition.build(B32:B38,C32:C38,F14:F27)</f>
-        <v>InterpolatedNodalCurveDefinition@2</v>
+        <v>InterpolatedNodalCurveDefinition@4</v>
       </c>
       <c r="H31" s="16" t="str">
         <f>_xll.og.InterpolatedNodalCurveDefinition.build(H32:H38,I32:I38,L14:L26)</f>
-        <v>InterpolatedNodalCurveDefinition@3</v>
+        <v>InterpolatedNodalCurveDefinition@5</v>
       </c>
       <c r="N31" s="16" t="str">
         <f>_xll.og.InterpolatedNodalCurveDefinition.build(N32:N38,O32:O38,R14:R25)</f>
-        <v>InterpolatedNodalCurveDefinition@1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.45">
+        <v>InterpolatedNodalCurveDefinition@6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>48</v>
       </c>
@@ -1668,7 +1667,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>50</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>58</v>
       </c>
@@ -1708,7 +1707,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>59</v>
       </c>
@@ -1728,7 +1727,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>53</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>56</v>
       </c>
@@ -1768,7 +1767,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>55</v>
       </c>
@@ -1788,21 +1787,21 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="16" t="str">
-        <f>_xll.og.CurveGroupEntry.of(C41,C42,C43)</f>
-        <v>CurveGroupEntry@1</v>
+        <f>_xll.og.RatesCurveGroupEntry.of(C41,C42,C43)</f>
+        <v>RatesCurveGroupEntry@4</v>
       </c>
       <c r="H40" s="16" t="str">
-        <f>_xll.og.CurveGroupEntry.of(I41,I42,I43)</f>
-        <v>CurveGroupEntry@3</v>
+        <f>_xll.og.RatesCurveGroupEntry.of(I41,I42,I43)</f>
+        <v>RatesCurveGroupEntry@5</v>
       </c>
       <c r="N40" s="16" t="str">
-        <f>_xll.og.CurveGroupEntry.of(O41,O42,O43)</f>
-        <v>CurveGroupEntry@2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.45">
+        <f>_xll.og.RatesCurveGroupEntry.of(O41,O42,O43)</f>
+        <v>RatesCurveGroupEntry@6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>48</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>12</v>
       </c>
@@ -1842,13 +1841,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C43" s="12" t="str">
         <f>_xll.og.OvernightIndex.of(D43)</f>
-        <v>ImmutableOvernightIndex@1</v>
+        <v>ImmutableOvernightIndex@2</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>62</v>
@@ -1858,7 +1857,7 @@
       </c>
       <c r="I43" s="12" t="str">
         <f>_xll.og.IborIndex.of(J43)</f>
-        <v>ImmutableIborIndex@2</v>
+        <v>ImmutableIborIndex@3</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>71</v>
@@ -1868,7 +1867,7 @@
       </c>
       <c r="O43" s="12" t="str">
         <f>_xll.og.IborIndex.of(P43)</f>
-        <v>ImmutableIborIndex@1</v>
+        <v>ImmutableIborIndex@4</v>
       </c>
       <c r="P43" s="4" t="s">
         <v>79</v>
@@ -1880,53 +1879,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.59765625" customWidth="1"/>
-    <col min="15" max="15" width="21.9296875" customWidth="1"/>
-    <col min="16" max="16" width="22.59765625" customWidth="1"/>
-    <col min="17" max="17" width="18.796875" customWidth="1"/>
-    <col min="18" max="18" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="22" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="28" customWidth="1"/>
     <col min="20" max="20" width="24" customWidth="1"/>
-    <col min="21" max="21" width="18.19921875" customWidth="1"/>
+    <col min="21" max="21" width="18.140625" customWidth="1"/>
     <col min="22" max="22" width="15" customWidth="1"/>
-    <col min="23" max="23" width="11.86328125" customWidth="1"/>
-    <col min="24" max="24" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.53125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="8" t="str">
         <f>_xll.og.ReferenceData.standard()</f>
-        <v>ImmutableReferenceData@1</v>
+        <v>ImmutableReferenceData@3</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>69</v>
       </c>
       <c r="F2" s="20" t="str">
         <f>_xll.og.DiscountingSwapProductPricer.DEFAULT()</f>
-        <v>DiscountingSwapProductPricer@1</v>
+        <v>DiscountingSwapProductPricer@2</v>
       </c>
       <c r="L2" s="19"/>
       <c r="M2" s="19" t="s">
@@ -1945,24 +1944,24 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="str">
         <f>_xll.og.Swap.resolve(C5,C2)</f>
-        <v>ResolvedSwap@1</v>
+        <v>ResolvedSwap@2</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F3" s="20" t="str">
         <f>_xll.og.DiscountingSwapProductPricer.presentValueMultiCurrency(F2,C3,'Market Data'!B2)</f>
-        <v>MultiCurrencyAmount@1</v>
+        <v>MultiCurrencyAmount@2</v>
       </c>
       <c r="L3" s="3" t="str">
         <f t="array" ref="L3:L18">_xll.og.List.explode(F5)</f>
-        <v>IborRateSensitivity@1</v>
+        <v>IborRateSensitivity@9</v>
       </c>
       <c r="M3" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L3,M$2))</f>
@@ -1985,7 +1984,7 @@
         <v>2556450.1789434357</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E4" s="19" t="s">
         <v>78</v>
       </c>
@@ -1994,7 +1993,7 @@
         <v>-272455.95127698663</v>
       </c>
       <c r="L4" s="3" t="str">
-        <v>IborRateSensitivity@2</v>
+        <v>IborRateSensitivity@10</v>
       </c>
       <c r="M4" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L4,M$2))</f>
@@ -2017,23 +2016,23 @@
         <v>2557326.0710469773</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="8" t="str">
         <f>_xll.og.Swap.of(C6:C7)</f>
-        <v>Swap@1</v>
+        <v>Swap@2</v>
       </c>
       <c r="E5" s="19" t="s">
         <v>87</v>
       </c>
       <c r="F5" s="21" t="str">
         <f>_xll.og.PointSensitivities.getSensitivities(_xll.og.PointSensitivities.normalized(_xll.og.PointSensitivityBuilder.build(_xll.og.DiscountingSwapProductPricer.presentValueSensitivity(F2,C3,'Market Data'!B2))))</f>
-        <v>RegularImmutableList@1</v>
+        <v>RegularImmutableList@2</v>
       </c>
       <c r="L5" s="3" t="str">
-        <v>IborRateSensitivity@3</v>
+        <v>IborRateSensitivity@11</v>
       </c>
       <c r="M5" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L5,M$2))</f>
@@ -2056,16 +2055,16 @@
         <v>2531429.3182908599</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>C9</f>
-        <v>RateCalculationSwapLeg@2</v>
+        <v>RateCalculationSwapLeg@4</v>
       </c>
       <c r="L6" s="3" t="str">
-        <v>IborRateSensitivity@4</v>
+        <v>IborRateSensitivity@12</v>
       </c>
       <c r="M6" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L6,M$2))</f>
@@ -2088,16 +2087,16 @@
         <v>2504777.6951774531</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>H9</f>
-        <v>RateCalculationSwapLeg@1</v>
+        <v>RateCalculationSwapLeg@3</v>
       </c>
       <c r="L7" s="3" t="str">
-        <v>IborRateSensitivity@5</v>
+        <v>IborRateSensitivity@13</v>
       </c>
       <c r="M7" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L7,M$2))</f>
@@ -2120,9 +2119,9 @@
         <v>2561913.0308725024</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="L8" s="3" t="str">
-        <v>IborRateSensitivity@6</v>
+        <v>IborRateSensitivity@14</v>
       </c>
       <c r="M8" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L8,M$2))</f>
@@ -2145,23 +2144,23 @@
         <v>2619250.9833476138</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="8" t="str">
         <f>_xll.og.RateCalculationSwapLeg.build(B10:B14,C10:C14)</f>
-        <v>RateCalculationSwapLeg@2</v>
+        <v>RateCalculationSwapLeg@4</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="8" t="str">
         <f>_xll.og.RateCalculationSwapLeg.build(G10:G14,H10:H14)</f>
-        <v>RateCalculationSwapLeg@1</v>
+        <v>RateCalculationSwapLeg@3</v>
       </c>
       <c r="L9" s="3" t="str">
-        <v>IborRateSensitivity@7</v>
+        <v>IborRateSensitivity@15</v>
       </c>
       <c r="M9" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L9,M$2))</f>
@@ -2184,7 +2183,7 @@
         <v>2537297.6014800463</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
@@ -2198,7 +2197,7 @@
         <v>20</v>
       </c>
       <c r="L10" s="3" t="str">
-        <v>IborRateSensitivity@8</v>
+        <v>IborRateSensitivity@16</v>
       </c>
       <c r="M10" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L10,M$2))</f>
@@ -2221,23 +2220,23 @@
         <v>2455273.4145536497</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>C16</f>
-        <v>PeriodicSchedule@2</v>
+        <v>PeriodicSchedule@3</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H11" s="1" t="str">
         <f>H16</f>
-        <v>PeriodicSchedule@1</v>
+        <v>PeriodicSchedule@4</v>
       </c>
       <c r="L11" s="3" t="str">
-        <v>ZeroRateSensitivity@1</v>
+        <v>ZeroRateSensitivity@9</v>
       </c>
       <c r="M11" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L11,M$2))</f>
@@ -2260,23 +2259,23 @@
         <v>7933.4003224362186</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="str">
         <f>C22</f>
-        <v>PaymentSchedule@1</v>
+        <v>PaymentSchedule@4</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="1" t="str">
         <f>H22</f>
-        <v>PaymentSchedule@2</v>
+        <v>PaymentSchedule@3</v>
       </c>
       <c r="L12" s="3" t="str">
-        <v>ZeroRateSensitivity@2</v>
+        <v>ZeroRateSensitivity@10</v>
       </c>
       <c r="M12" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L12,M$2))</f>
@@ -2299,23 +2298,23 @@
         <v>17071.727958181815</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>_xll.og.NotionalSchedule.build(B27:B28,C27:C28)</f>
-        <v>NotionalSchedule@1</v>
+        <v>NotionalSchedule@4</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="1" t="str">
         <f>H26</f>
-        <v>NotionalSchedule@2</v>
+        <v>NotionalSchedule@6</v>
       </c>
       <c r="L13" s="3" t="str">
-        <v>ZeroRateSensitivity@3</v>
+        <v>ZeroRateSensitivity@11</v>
       </c>
       <c r="M13" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L13,M$2))</f>
@@ -2338,13 +2337,13 @@
         <v>25166.568677485251</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>_xll.og.FixedRateCalculation.of(D14,E14)</f>
-        <v>FixedRateCalculation@1</v>
+        <v>FixedRateCalculation@2</v>
       </c>
       <c r="D14" s="7">
         <v>0.01</v>
@@ -2357,13 +2356,13 @@
       </c>
       <c r="H14" s="1" t="str">
         <f>_xll.og.IborRateCalculation.of(I14)</f>
-        <v>IborRateCalculation@1</v>
+        <v>IborRateCalculation@2</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>71</v>
       </c>
       <c r="L14" s="3" t="str">
-        <v>ZeroRateSensitivity@4</v>
+        <v>ZeroRateSensitivity@12</v>
       </c>
       <c r="M14" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L14,M$2))</f>
@@ -2386,9 +2385,9 @@
         <v>35787.13660480408</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="L15" s="3" t="str">
-        <v>ZeroRateSensitivity@5</v>
+        <v>ZeroRateSensitivity@13</v>
       </c>
       <c r="M15" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L15,M$2))</f>
@@ -2411,23 +2410,23 @@
         <v>43439.604779939771</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="8" t="str">
         <f>_xll.og.PeriodicSchedule.build(B17:B20,C17:C20)</f>
-        <v>PeriodicSchedule@2</v>
+        <v>PeriodicSchedule@3</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="8" t="str">
         <f>_xll.og.PeriodicSchedule.build(G17:G20,H17:H20)</f>
-        <v>PeriodicSchedule@1</v>
+        <v>PeriodicSchedule@4</v>
       </c>
       <c r="L16" s="3" t="str">
-        <v>ZeroRateSensitivity@6</v>
+        <v>ZeroRateSensitivity@14</v>
       </c>
       <c r="M16" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L16,M$2))</f>
@@ -2450,7 +2449,7 @@
         <v>54118.288769099832</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
@@ -2464,7 +2463,7 @@
         <v>42431</v>
       </c>
       <c r="L17" s="3" t="str">
-        <v>ZeroRateSensitivity@7</v>
+        <v>ZeroRateSensitivity@15</v>
       </c>
       <c r="M17" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L17,M$2))</f>
@@ -2487,7 +2486,7 @@
         <v>61738.114744073675</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
@@ -2501,7 +2500,7 @@
         <v>43161</v>
       </c>
       <c r="L18" s="3" t="str">
-        <v>ZeroRateSensitivity@8</v>
+        <v>ZeroRateSensitivity@16</v>
       </c>
       <c r="M18" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L18,M$2))</f>
@@ -2524,7 +2523,7 @@
         <v>68469.259415752371</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
@@ -2538,13 +2537,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="1" t="str">
         <f>_xll.og.BusinessDayAdjustment.of(D20,E20)</f>
-        <v>BusinessDayAdjustment@1</v>
+        <v>BusinessDayAdjustment@3</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>7</v>
@@ -2557,7 +2556,7 @@
       </c>
       <c r="H20" s="1" t="str">
         <f>_xll.og.BusinessDayAdjustment.of(I20,J20)</f>
-        <v>BusinessDayAdjustment@2</v>
+        <v>BusinessDayAdjustment@4</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>7</v>
@@ -2566,25 +2565,25 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="8" t="str">
         <f>_xll.og.PaymentSchedule.build(B23:B24,C23:C24)</f>
-        <v>PaymentSchedule@1</v>
+        <v>PaymentSchedule@4</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H22" s="8" t="str">
         <f>_xll.og.PaymentSchedule.build(G23:G24,H23:H24)</f>
-        <v>PaymentSchedule@2</v>
+        <v>PaymentSchedule@3</v>
       </c>
       <c r="O22" s="22"/>
       <c r="Q22" s="6"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
@@ -2600,7 +2599,7 @@
       <c r="O23" s="22"/>
       <c r="Q23" s="6"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>9</v>
       </c>
@@ -2616,29 +2615,29 @@
       <c r="O24" s="22"/>
       <c r="Q24" s="6"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="O25" s="22"/>
       <c r="Q25" s="6"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="8" t="str">
         <f>_xll.og.NotionalSchedule.build(B27:B28,C27:C28)</f>
-        <v>NotionalSchedule@3</v>
+        <v>NotionalSchedule@5</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H26" s="8" t="str">
         <f>_xll.og.NotionalSchedule.build(G27:G28,H27:H28)</f>
-        <v>NotionalSchedule@2</v>
+        <v>NotionalSchedule@6</v>
       </c>
       <c r="O26" s="22"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>12</v>
       </c>
@@ -2654,7 +2653,7 @@
       <c r="O27" s="22"/>
       <c r="Q27" s="6"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>13</v>
       </c>
@@ -2671,7 +2670,7 @@
       <c r="O28" s="22"/>
       <c r="Q28" s="6"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="O29" s="22"/>
       <c r="Q29" s="6"/>
     </row>

</xml_diff>

<commit_message>
Update wrappers for Strata v2.11.5
</commit_message>
<xml_diff>
--- a/examples/swap-pricer.xlsx
+++ b/examples/swap-pricer.xlsx
@@ -1,25 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\strata-excel\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E3A67379-4C00-483A-ADC6-FE37DCAED699}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ED1750-BA99-46DA-8E41-7CB27C6FDFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="3960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5450" yWindow="3620" windowWidth="32950" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Market Data" sheetId="2" r:id="rId1"/>
     <sheet name="Swap" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -780,35 +790,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:R43"/>
+  <dimension ref="B2:R47"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" customWidth="1"/>
+    <col min="2" max="5" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B2" s="16" t="str">
         <f>_xll.og.RatesCurveCalibrator.calibrate(_xll.og.RatesCurveCalibrator.standard(),B8,C4,C6)</f>
-        <v>ImmutableRatesProvider@2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'com.opengamma.strata.market.curve.RatesCurveGroupDefinition'</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>67</v>
       </c>
@@ -816,48 +828,48 @@
         <v>42429</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="17" t="str">
         <f>_xll.og.MarketData.combinedWith(_xll.og.MarketData.combinedWith(C5,D5),E5)</f>
-        <v>ImmutableMarketData@10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>ImmutableMarketData@5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C5" s="12" t="str">
         <f>_xll.og.MarketData.of(C3,E14:E27,D14:D27)</f>
-        <v>ImmutableMarketData@6</v>
+        <v>ImmutableMarketData@2</v>
       </c>
       <c r="D5" s="12" t="str">
         <f>_xll.og.MarketData.of(C3,K14:K26,J14:J26)</f>
-        <v>ImmutableMarketData@8</v>
+        <v>ImmutableMarketData@3</v>
       </c>
       <c r="E5" s="12" t="str">
         <f>_xll.og.MarketData.of(C3,Q14:Q25,P14:P25)</f>
-        <v>ImmutableMarketData@7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+        <v>ImmutableMarketData@1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="12" t="str">
         <f>_xll.og.ReferenceData.standard()</f>
-        <v>ImmutableReferenceData@4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+        <v>ImmutableReferenceData@2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B8" s="16" t="str">
         <f>_xll.og.RatesCurveGroupDefinition.of(C9,C10:E10,C11:E11)</f>
-        <v>RatesCurveGroupDefinition@2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+        <v>## com/opengamma/strata/market/curve/RatesCurveGroupEntry</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>48</v>
       </c>
@@ -865,41 +877,41 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="12" t="str">
         <f>B40</f>
-        <v>RatesCurveGroupEntry@4</v>
+        <v>## com/opengamma/strata/basics/currency/Currency</v>
       </c>
       <c r="D10" s="12" t="str">
         <f>H40</f>
-        <v>RatesCurveGroupEntry@5</v>
+        <v>## com/opengamma/strata/basics/currency/Currency</v>
       </c>
       <c r="E10" s="12" t="str">
         <f>N40</f>
-        <v>RatesCurveGroupEntry@6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+        <v>## com/opengamma/strata/basics/currency/Currency</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C11" s="12" t="str">
         <f>B31</f>
-        <v>InterpolatedNodalCurveDefinition@4</v>
+        <v>InterpolatedNodalCurveDefinition@2</v>
       </c>
       <c r="D11" s="12" t="str">
         <f>H31</f>
-        <v>InterpolatedNodalCurveDefinition@5</v>
+        <v>InterpolatedNodalCurveDefinition@1</v>
       </c>
       <c r="E11" s="12" t="str">
         <f>N31</f>
-        <v>InterpolatedNodalCurveDefinition@6</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+        <v>InterpolatedNodalCurveDefinition@3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
@@ -946,7 +958,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B14" s="12" t="s">
         <v>29</v>
       </c>
@@ -958,11 +970,11 @@
       </c>
       <c r="E14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B14&amp;"."&amp;C14)</f>
-        <v>QuoteId@41</v>
+        <v>QuoteId@4</v>
       </c>
       <c r="F14" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C14,B14),E14)</f>
-        <v>FixedOvernightSwapCurveNode@28</v>
+        <v>FixedOvernightSwapCurveNode@14</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>71</v>
@@ -973,11 +985,11 @@
       </c>
       <c r="K14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H14&amp;"."&amp;I14)</f>
-        <v>QuoteId@40</v>
+        <v>QuoteId@1</v>
       </c>
       <c r="L14" s="13" t="str">
         <f>_xll.og.IborFixingDepositCurveNode.ofRate( _xll.og.IborFixingDepositTemplate.of(H14),K14)</f>
-        <v>IborFixingDepositCurveNode@3</v>
+        <v>IborFixingDepositCurveNode@1</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>79</v>
@@ -988,14 +1000,14 @@
       </c>
       <c r="Q14" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N14&amp;"."&amp;O14)</f>
-        <v>QuoteId@42</v>
+        <v>QuoteId@3</v>
       </c>
       <c r="R14" s="13" t="str">
         <f>_xll.og.IborFixingDepositCurveNode.ofRate( _xll.og.IborFixingDepositTemplate.of(N14),Q14)</f>
-        <v>IborFixingDepositCurveNode@4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+        <v>IborFixingDepositCurveNode@2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B15" s="12" t="s">
         <v>29</v>
       </c>
@@ -1007,11 +1019,11 @@
       </c>
       <c r="E15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B15&amp;"."&amp;C15)</f>
-        <v>QuoteId@49</v>
+        <v>QuoteId@2</v>
       </c>
       <c r="F15" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C15,B15),E15)</f>
-        <v>FixedOvernightSwapCurveNode@17</v>
+        <v>FixedOvernightSwapCurveNode@4</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>71</v>
@@ -1024,11 +1036,11 @@
       </c>
       <c r="K15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H15&amp;"."&amp;I15)</f>
-        <v>QuoteId@43</v>
+        <v>QuoteId@15</v>
       </c>
       <c r="L15" s="13" t="str">
         <f>_xll.og.FraCurveNode.ofRate(_xll.og.FraTemplate.ofIndex(I15,H15),K15)</f>
-        <v>FraCurveNode@5</v>
+        <v>FraCurveNode@1</v>
       </c>
       <c r="N15" s="12" t="s">
         <v>79</v>
@@ -1041,14 +1053,14 @@
       </c>
       <c r="Q15" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N15&amp;"."&amp;O15)</f>
-        <v>QuoteId@44</v>
+        <v>QuoteId@5</v>
       </c>
       <c r="R15" s="13" t="str">
         <f>_xll.og.FraCurveNode.ofRate(_xll.og.FraTemplate.ofIndex(O15,N15),Q15)</f>
-        <v>FraCurveNode@4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FraCurveNode@3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B16" s="12" t="s">
         <v>29</v>
       </c>
@@ -1060,11 +1072,11 @@
       </c>
       <c r="E16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B16&amp;"."&amp;C16)</f>
-        <v>QuoteId@45</v>
+        <v>QuoteId@7</v>
       </c>
       <c r="F16" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C16,B16),E16)</f>
-        <v>FixedOvernightSwapCurveNode@15</v>
+        <v>FixedOvernightSwapCurveNode@3</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>71</v>
@@ -1077,11 +1089,11 @@
       </c>
       <c r="K16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H16&amp;"."&amp;I16)</f>
-        <v>QuoteId@52</v>
+        <v>QuoteId@10</v>
       </c>
       <c r="L16" s="13" t="str">
         <f>_xll.og.FraCurveNode.ofRate(_xll.og.FraTemplate.ofIndex(I16,H16),K16)</f>
-        <v>FraCurveNode@6</v>
+        <v>FraCurveNode@2</v>
       </c>
       <c r="N16" s="12" t="s">
         <v>80</v>
@@ -1094,14 +1106,14 @@
       </c>
       <c r="Q16" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N16&amp;"."&amp;O16)</f>
-        <v>QuoteId@47</v>
+        <v>QuoteId@17</v>
       </c>
       <c r="R16" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O16,N16),Q16)</f>
-        <v>FixedIborSwapCurveNode@21</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FixedIborSwapCurveNode@3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B17" s="12" t="s">
         <v>29</v>
       </c>
@@ -1113,11 +1125,11 @@
       </c>
       <c r="E17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B17&amp;"."&amp;C17)</f>
-        <v>QuoteId@46</v>
+        <v>QuoteId@13</v>
       </c>
       <c r="F17" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C17,B17),E17)</f>
-        <v>FixedOvernightSwapCurveNode@16</v>
+        <v>FixedOvernightSwapCurveNode@5</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>75</v>
@@ -1130,11 +1142,11 @@
       </c>
       <c r="K17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H17&amp;"."&amp;I17)</f>
-        <v>QuoteId@48</v>
+        <v>QuoteId@14</v>
       </c>
       <c r="L17" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I17,H17),K17)</f>
-        <v>FixedIborSwapCurveNode@22</v>
+        <v>FixedIborSwapCurveNode@1</v>
       </c>
       <c r="N17" s="12" t="s">
         <v>80</v>
@@ -1147,14 +1159,14 @@
       </c>
       <c r="Q17" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N17&amp;"."&amp;O17)</f>
-        <v>QuoteId@58</v>
+        <v>QuoteId@12</v>
       </c>
       <c r="R17" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O17,N17),Q17)</f>
-        <v>FixedIborSwapCurveNode@27</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FixedIborSwapCurveNode@4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B18" s="12" t="s">
         <v>29</v>
       </c>
@@ -1166,11 +1178,11 @@
       </c>
       <c r="E18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B18&amp;"."&amp;C18)</f>
-        <v>QuoteId@55</v>
+        <v>QuoteId@11</v>
       </c>
       <c r="F18" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C18,B18),E18)</f>
-        <v>FixedOvernightSwapCurveNode@19</v>
+        <v>FixedOvernightSwapCurveNode@6</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>75</v>
@@ -1183,11 +1195,11 @@
       </c>
       <c r="K18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H18&amp;"."&amp;I18)</f>
-        <v>QuoteId@51</v>
+        <v>QuoteId@9</v>
       </c>
       <c r="L18" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I18,H18),K18)</f>
-        <v>FixedIborSwapCurveNode@24</v>
+        <v>FixedIborSwapCurveNode@9</v>
       </c>
       <c r="N18" s="12" t="s">
         <v>80</v>
@@ -1200,14 +1212,14 @@
       </c>
       <c r="Q18" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N18&amp;"."&amp;O18)</f>
-        <v>QuoteId@50</v>
+        <v>QuoteId@8</v>
       </c>
       <c r="R18" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O18,N18),Q18)</f>
-        <v>FixedIborSwapCurveNode@23</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FixedIborSwapCurveNode@5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B19" s="12" t="s">
         <v>29</v>
       </c>
@@ -1219,11 +1231,11 @@
       </c>
       <c r="E19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B19&amp;"."&amp;C19)</f>
-        <v>QuoteId@62</v>
+        <v>QuoteId@16</v>
       </c>
       <c r="F19" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C19,B19),E19)</f>
-        <v>FixedOvernightSwapCurveNode@23</v>
+        <v>FixedOvernightSwapCurveNode@7</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>75</v>
@@ -1236,11 +1248,11 @@
       </c>
       <c r="K19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H19&amp;"."&amp;I19)</f>
-        <v>QuoteId@59</v>
+        <v>QuoteId@6</v>
       </c>
       <c r="L19" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I19,H19),K19)</f>
-        <v>FixedIborSwapCurveNode@29</v>
+        <v>FixedIborSwapCurveNode@7</v>
       </c>
       <c r="N19" s="12" t="s">
         <v>80</v>
@@ -1253,14 +1265,14 @@
       </c>
       <c r="Q19" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N19&amp;"."&amp;O19)</f>
-        <v>QuoteId@54</v>
+        <v>QuoteId@33</v>
       </c>
       <c r="R19" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O19,N19),Q19)</f>
-        <v>FixedIborSwapCurveNode@25</v>
-      </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FixedIborSwapCurveNode@16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B20" s="12" t="s">
         <v>29</v>
       </c>
@@ -1272,11 +1284,11 @@
       </c>
       <c r="E20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B20&amp;"."&amp;C20)</f>
-        <v>QuoteId@53</v>
+        <v>QuoteId@28</v>
       </c>
       <c r="F20" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C20,B20),E20)</f>
-        <v>FixedOvernightSwapCurveNode@18</v>
+        <v>FixedOvernightSwapCurveNode@10</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>75</v>
@@ -1289,11 +1301,11 @@
       </c>
       <c r="K20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H20&amp;"."&amp;I20)</f>
-        <v>QuoteId@71</v>
+        <v>QuoteId@29</v>
       </c>
       <c r="L20" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I20,H20),K20)</f>
-        <v>FixedIborSwapCurveNode@35</v>
+        <v>FixedIborSwapCurveNode@17</v>
       </c>
       <c r="N20" s="12" t="s">
         <v>80</v>
@@ -1306,14 +1318,14 @@
       </c>
       <c r="Q20" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N20&amp;"."&amp;O20)</f>
-        <v>QuoteId@63</v>
+        <v>QuoteId@36</v>
       </c>
       <c r="R20" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O20,N20),Q20)</f>
-        <v>FixedIborSwapCurveNode@31</v>
-      </c>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FixedIborSwapCurveNode@20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B21" s="12" t="s">
         <v>29</v>
       </c>
@@ -1325,11 +1337,11 @@
       </c>
       <c r="E21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B21&amp;"."&amp;C21)</f>
-        <v>QuoteId@57</v>
+        <v>QuoteId@37</v>
       </c>
       <c r="F21" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C21,B21),E21)</f>
-        <v>FixedOvernightSwapCurveNode@20</v>
+        <v>FixedOvernightSwapCurveNode@12</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>75</v>
@@ -1342,11 +1354,11 @@
       </c>
       <c r="K21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H21&amp;"."&amp;I21)</f>
-        <v>QuoteId@56</v>
+        <v>QuoteId@25</v>
       </c>
       <c r="L21" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I21,H21),K21)</f>
-        <v>FixedIborSwapCurveNode@26</v>
+        <v>FixedIborSwapCurveNode@10</v>
       </c>
       <c r="N21" s="12" t="s">
         <v>80</v>
@@ -1359,14 +1371,14 @@
       </c>
       <c r="Q21" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N21&amp;"."&amp;O21)</f>
-        <v>QuoteId@73</v>
+        <v>QuoteId@38</v>
       </c>
       <c r="R21" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O21,N21),Q21)</f>
-        <v>FixedIborSwapCurveNode@37</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FixedIborSwapCurveNode@19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B22" s="12" t="s">
         <v>29</v>
       </c>
@@ -1378,11 +1390,11 @@
       </c>
       <c r="E22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B22&amp;"."&amp;C22)</f>
-        <v>QuoteId@67</v>
+        <v>QuoteId@20</v>
       </c>
       <c r="F22" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C22,B22),E22)</f>
-        <v>FixedOvernightSwapCurveNode@22</v>
+        <v>FixedOvernightSwapCurveNode@2</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>75</v>
@@ -1395,11 +1407,11 @@
       </c>
       <c r="K22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H22&amp;"."&amp;I22)</f>
-        <v>QuoteId@61</v>
+        <v>QuoteId@26</v>
       </c>
       <c r="L22" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I22,H22),K22)</f>
-        <v>FixedIborSwapCurveNode@30</v>
+        <v>FixedIborSwapCurveNode@15</v>
       </c>
       <c r="N22" s="12" t="s">
         <v>80</v>
@@ -1412,14 +1424,14 @@
       </c>
       <c r="Q22" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N22&amp;"."&amp;O22)</f>
-        <v>QuoteId@60</v>
+        <v>QuoteId@18</v>
       </c>
       <c r="R22" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O22,N22),Q22)</f>
-        <v>FixedIborSwapCurveNode@28</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FixedIborSwapCurveNode@2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B23" s="12" t="s">
         <v>29</v>
       </c>
@@ -1431,11 +1443,11 @@
       </c>
       <c r="E23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B23&amp;"."&amp;C23)</f>
-        <v>QuoteId@76</v>
+        <v>QuoteId@19</v>
       </c>
       <c r="F23" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C23,B23),E23)</f>
-        <v>FixedOvernightSwapCurveNode@26</v>
+        <v>FixedOvernightSwapCurveNode@1</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>75</v>
@@ -1448,11 +1460,11 @@
       </c>
       <c r="K23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H23&amp;"."&amp;I23)</f>
-        <v>QuoteId@70</v>
+        <v>QuoteId@21</v>
       </c>
       <c r="L23" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I23,H23),K23)</f>
-        <v>FixedIborSwapCurveNode@34</v>
+        <v>FixedIborSwapCurveNode@6</v>
       </c>
       <c r="N23" s="12" t="s">
         <v>80</v>
@@ -1465,14 +1477,14 @@
       </c>
       <c r="Q23" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N23&amp;"."&amp;O23)</f>
-        <v>QuoteId@65</v>
+        <v>QuoteId@22</v>
       </c>
       <c r="R23" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O23,N23),Q23)</f>
-        <v>FixedIborSwapCurveNode@32</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FixedIborSwapCurveNode@8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B24" s="12" t="s">
         <v>29</v>
       </c>
@@ -1484,11 +1496,11 @@
       </c>
       <c r="E24" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B24&amp;"."&amp;C24)</f>
-        <v>QuoteId@64</v>
+        <v>QuoteId@23</v>
       </c>
       <c r="F24" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C24,B24),E24)</f>
-        <v>FixedOvernightSwapCurveNode@21</v>
+        <v>FixedOvernightSwapCurveNode@8</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>75</v>
@@ -1501,11 +1513,11 @@
       </c>
       <c r="K24" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H24&amp;"."&amp;I24)</f>
-        <v>QuoteId@74</v>
+        <v>QuoteId@24</v>
       </c>
       <c r="L24" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I24,H24),K24)</f>
-        <v>FixedIborSwapCurveNode@38</v>
+        <v>FixedIborSwapCurveNode@13</v>
       </c>
       <c r="N24" s="12" t="s">
         <v>80</v>
@@ -1518,14 +1530,14 @@
       </c>
       <c r="Q24" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N24&amp;"."&amp;O24)</f>
-        <v>QuoteId@72</v>
+        <v>QuoteId@31</v>
       </c>
       <c r="R24" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O24,N24),Q24)</f>
-        <v>FixedIborSwapCurveNode@36</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FixedIborSwapCurveNode@11</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B25" s="12" t="s">
         <v>29</v>
       </c>
@@ -1537,11 +1549,11 @@
       </c>
       <c r="E25" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B25&amp;"."&amp;C25)</f>
-        <v>QuoteId@68</v>
+        <v>QuoteId@27</v>
       </c>
       <c r="F25" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C25,B25),E25)</f>
-        <v>FixedOvernightSwapCurveNode@24</v>
+        <v>FixedOvernightSwapCurveNode@9</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>75</v>
@@ -1554,11 +1566,11 @@
       </c>
       <c r="K25" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H25&amp;"."&amp;I25)</f>
-        <v>QuoteId@66</v>
+        <v>QuoteId@30</v>
       </c>
       <c r="L25" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I25,H25),K25)</f>
-        <v>FixedIborSwapCurveNode@33</v>
+        <v>FixedIborSwapCurveNode@14</v>
       </c>
       <c r="N25" s="12" t="s">
         <v>80</v>
@@ -1571,14 +1583,14 @@
       </c>
       <c r="Q25" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;N25&amp;"."&amp;O25)</f>
-        <v>QuoteId@77</v>
+        <v>QuoteId@32</v>
       </c>
       <c r="R25" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(O25,N25),Q25)</f>
-        <v>FixedIborSwapCurveNode@39</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FixedIborSwapCurveNode@12</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B26" s="12" t="s">
         <v>29</v>
       </c>
@@ -1590,11 +1602,11 @@
       </c>
       <c r="E26" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B26&amp;"."&amp;C26)</f>
-        <v>QuoteId@75</v>
+        <v>QuoteId@34</v>
       </c>
       <c r="F26" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C26,B26),E26)</f>
-        <v>FixedOvernightSwapCurveNode@27</v>
+        <v>FixedOvernightSwapCurveNode@11</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>75</v>
@@ -1607,14 +1619,14 @@
       </c>
       <c r="K26" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;H26&amp;"."&amp;I26)</f>
-        <v>QuoteId@78</v>
+        <v>QuoteId@39</v>
       </c>
       <c r="L26" s="13" t="str">
         <f>_xll.og.FixedIborSwapCurveNode.ofRate(_xll.og.FixedIborSwapTemplate.of(I26,H26),K26)</f>
-        <v>FixedIborSwapCurveNode@40</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FixedIborSwapCurveNode@18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B27" s="12" t="s">
         <v>29</v>
       </c>
@@ -1626,28 +1638,28 @@
       </c>
       <c r="E27" s="13" t="str">
         <f>_xll.og.QuoteId.of("Excel~" &amp;B27&amp;"."&amp;C27)</f>
-        <v>QuoteId@69</v>
+        <v>QuoteId@35</v>
       </c>
       <c r="F27" s="13" t="str">
         <f>_xll.og.FixedOvernightSwapCurveNode.ofRate(_xll.og.FixedOvernightSwapTemplate.of(C27,B27),E27)</f>
-        <v>FixedOvernightSwapCurveNode@25</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+        <v>FixedOvernightSwapCurveNode@13</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B31" s="16" t="str">
         <f>_xll.og.InterpolatedNodalCurveDefinition.build(B32:B38,C32:C38,F14:F27)</f>
-        <v>InterpolatedNodalCurveDefinition@4</v>
+        <v>InterpolatedNodalCurveDefinition@2</v>
       </c>
       <c r="H31" s="16" t="str">
         <f>_xll.og.InterpolatedNodalCurveDefinition.build(H32:H38,I32:I38,L14:L26)</f>
-        <v>InterpolatedNodalCurveDefinition@5</v>
+        <v>InterpolatedNodalCurveDefinition@1</v>
       </c>
       <c r="N31" s="16" t="str">
         <f>_xll.og.InterpolatedNodalCurveDefinition.build(N32:N38,O32:O38,R14:R25)</f>
-        <v>InterpolatedNodalCurveDefinition@6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+        <v>InterpolatedNodalCurveDefinition@3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
         <v>48</v>
       </c>
@@ -1667,7 +1679,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
         <v>50</v>
       </c>
@@ -1687,7 +1699,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
         <v>58</v>
       </c>
@@ -1707,7 +1719,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>59</v>
       </c>
@@ -1727,7 +1739,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>53</v>
       </c>
@@ -1747,7 +1759,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
         <v>56</v>
       </c>
@@ -1767,7 +1779,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
         <v>55</v>
       </c>
@@ -1787,21 +1799,21 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B40" s="16" t="str">
         <f>_xll.og.RatesCurveGroupEntry.of(C41,C42,C43)</f>
-        <v>RatesCurveGroupEntry@4</v>
+        <v>## com/opengamma/strata/basics/currency/Currency</v>
       </c>
       <c r="H40" s="16" t="str">
         <f>_xll.og.RatesCurveGroupEntry.of(I41,I42,I43)</f>
-        <v>RatesCurveGroupEntry@5</v>
+        <v>## com/opengamma/strata/basics/currency/Currency</v>
       </c>
       <c r="N40" s="16" t="str">
         <f>_xll.og.RatesCurveGroupEntry.of(O41,O42,O43)</f>
-        <v>RatesCurveGroupEntry@6</v>
-      </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+        <v>## com/opengamma/strata/basics/currency/Currency</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
         <v>48</v>
       </c>
@@ -1821,7 +1833,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
         <v>12</v>
       </c>
@@ -1841,13 +1853,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C43" s="12" t="str">
         <f>_xll.og.OvernightIndex.of(D43)</f>
-        <v>ImmutableOvernightIndex@2</v>
+        <v>ImmutableOvernightIndex@1</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>62</v>
@@ -1857,7 +1869,7 @@
       </c>
       <c r="I43" s="12" t="str">
         <f>_xll.og.IborIndex.of(J43)</f>
-        <v>ImmutableIborIndex@3</v>
+        <v>ImmutableIborIndex@1</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>71</v>
@@ -1867,10 +1879,16 @@
       </c>
       <c r="O43" s="12" t="str">
         <f>_xll.og.IborIndex.of(P43)</f>
-        <v>ImmutableIborIndex@4</v>
+        <v>ImmutableIborIndex@2</v>
       </c>
       <c r="P43" s="4" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B47" t="str">
+        <f>_xll.og.RatesCurveGroupEntry.of(C41,C42,C43)</f>
+        <v>## com/opengamma/strata/basics/currency/Currency</v>
       </c>
     </row>
   </sheetData>
@@ -1882,50 +1900,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.54296875" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
-    <col min="16" max="16" width="22.5703125" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.54296875" customWidth="1"/>
+    <col min="17" max="17" width="18.81640625" customWidth="1"/>
+    <col min="18" max="18" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="28" customWidth="1"/>
     <col min="20" max="20" width="24" customWidth="1"/>
-    <col min="21" max="21" width="18.140625" customWidth="1"/>
+    <col min="21" max="21" width="18.1796875" customWidth="1"/>
     <col min="22" max="22" width="15" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" customWidth="1"/>
-    <col min="24" max="24" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.81640625" customWidth="1"/>
+    <col min="24" max="24" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B2" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="8" t="str">
         <f>_xll.og.ReferenceData.standard()</f>
-        <v>ImmutableReferenceData@3</v>
+        <v>ImmutableReferenceData@1</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>69</v>
       </c>
       <c r="F2" s="20" t="str">
         <f>_xll.og.DiscountingSwapProductPricer.DEFAULT()</f>
-        <v>DiscountingSwapProductPricer@2</v>
+        <v>DiscountingSwapProductPricer@1</v>
       </c>
       <c r="L2" s="19"/>
       <c r="M2" s="19" t="s">
@@ -1944,246 +1962,246 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="8" t="str">
         <f>_xll.og.Swap.resolve(C5,C2)</f>
-        <v>ResolvedSwap@2</v>
+        <v>ResolvedSwap@1</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F3" s="20" t="str">
         <f>_xll.og.DiscountingSwapProductPricer.presentValueMultiCurrency(F2,C3,'Market Data'!B2)</f>
-        <v>MultiCurrencyAmount@2</v>
+        <v>## Unable to convert argument to 'com.opengamma.strata.pricer.rate.RatesProvider'</v>
       </c>
       <c r="L3" s="3" t="str">
         <f t="array" ref="L3:L18">_xll.og.List.explode(F5)</f>
-        <v>IborRateSensitivity@9</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M3" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L3,M$2))</f>
-        <v>EUR</v>
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
       </c>
       <c r="N3" s="20" t="str">
         <f>_xll.og.Bean.property($L3,N$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O3" s="23" t="str">
         <f>_xll.og.Bean.property($L3,O$2)</f>
-        <v>EUR-EURIBOR-3M</v>
-      </c>
-      <c r="P3" s="20">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="P3" s="20" t="str">
         <f>_xll.og.Bean.property($L3,P$2)</f>
-        <v>0.25555555555555554</v>
-      </c>
-      <c r="Q3" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q3" s="24" t="str">
         <f>_xll.og.Bean.property($L3,Q$2)</f>
-        <v>2556450.1789434357</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
       <c r="E4" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="21" t="str">
         <f>_xll.og.CurrencyAmount.getAmount(_xll.og.MultiCurrencyAmount.getAmountOrZero(F3,"EUR"))</f>
-        <v>-272455.95127698663</v>
+        <v>## Unable to parse amount: ## com/opengamma/strata/basics/currency/CurrencyAmount</v>
       </c>
       <c r="L4" s="3" t="str">
-        <v>IborRateSensitivity@10</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M4" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L4,M$2))</f>
-        <v>EUR</v>
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
       </c>
       <c r="N4" s="20" t="str">
         <f>_xll.og.Bean.property($L4,N$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O4" s="23" t="str">
         <f>_xll.og.Bean.property($L4,O$2)</f>
-        <v>EUR-EURIBOR-3M</v>
-      </c>
-      <c r="P4" s="20">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="P4" s="20" t="str">
         <f>_xll.og.Bean.property($L4,P$2)</f>
-        <v>0.25555555555555554</v>
-      </c>
-      <c r="Q4" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q4" s="24" t="str">
         <f>_xll.og.Bean.property($L4,Q$2)</f>
-        <v>2557326.0710469773</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="8" t="str">
         <f>_xll.og.Swap.of(C6:C7)</f>
-        <v>Swap@2</v>
+        <v>Swap@1</v>
       </c>
       <c r="E5" s="19" t="s">
         <v>87</v>
       </c>
       <c r="F5" s="21" t="str">
         <f>_xll.og.PointSensitivities.getSensitivities(_xll.og.PointSensitivities.normalized(_xll.og.PointSensitivityBuilder.build(_xll.og.DiscountingSwapProductPricer.presentValueSensitivity(F2,C3,'Market Data'!B2))))</f>
-        <v>RegularImmutableList@2</v>
+        <v>## com/opengamma/strata/market/sensitivity/PointSensitivity</v>
       </c>
       <c r="L5" s="3" t="str">
-        <v>IborRateSensitivity@11</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M5" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L5,M$2))</f>
-        <v>EUR</v>
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
       </c>
       <c r="N5" s="20" t="str">
         <f>_xll.og.Bean.property($L5,N$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O5" s="23" t="str">
         <f>_xll.og.Bean.property($L5,O$2)</f>
-        <v>EUR-EURIBOR-3M</v>
-      </c>
-      <c r="P5" s="20">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="P5" s="20" t="str">
         <f>_xll.og.Bean.property($L5,P$2)</f>
-        <v>0.25277777777777777</v>
-      </c>
-      <c r="Q5" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q5" s="24" t="str">
         <f>_xll.og.Bean.property($L5,Q$2)</f>
-        <v>2531429.3182908599</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>C9</f>
-        <v>RateCalculationSwapLeg@4</v>
+        <v>RateCalculationSwapLeg@1</v>
       </c>
       <c r="L6" s="3" t="str">
-        <v>IborRateSensitivity@12</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M6" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L6,M$2))</f>
-        <v>EUR</v>
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
       </c>
       <c r="N6" s="20" t="str">
         <f>_xll.og.Bean.property($L6,N$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O6" s="23" t="str">
         <f>_xll.og.Bean.property($L6,O$2)</f>
-        <v>EUR-EURIBOR-3M</v>
-      </c>
-      <c r="P6" s="20">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="P6" s="20" t="str">
         <f>_xll.og.Bean.property($L6,P$2)</f>
-        <v>0.25</v>
-      </c>
-      <c r="Q6" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q6" s="24" t="str">
         <f>_xll.og.Bean.property($L6,Q$2)</f>
-        <v>2504777.6951774531</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>H9</f>
-        <v>RateCalculationSwapLeg@3</v>
+        <v>RateCalculationSwapLeg@2</v>
       </c>
       <c r="L7" s="3" t="str">
-        <v>IborRateSensitivity@13</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M7" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L7,M$2))</f>
-        <v>EUR</v>
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
       </c>
       <c r="N7" s="20" t="str">
         <f>_xll.og.Bean.property($L7,N$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O7" s="23" t="str">
         <f>_xll.og.Bean.property($L7,O$2)</f>
-        <v>EUR-EURIBOR-3M</v>
-      </c>
-      <c r="P7" s="20">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="P7" s="20" t="str">
         <f>_xll.og.Bean.property($L7,P$2)</f>
-        <v>0.25555555555555554</v>
-      </c>
-      <c r="Q7" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q7" s="24" t="str">
         <f>_xll.og.Bean.property($L7,Q$2)</f>
-        <v>2561913.0308725024</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="L8" s="3" t="str">
-        <v>IborRateSensitivity@14</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M8" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L8,M$2))</f>
-        <v>EUR</v>
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
       </c>
       <c r="N8" s="20" t="str">
         <f>_xll.og.Bean.property($L8,N$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O8" s="23" t="str">
         <f>_xll.og.Bean.property($L8,O$2)</f>
-        <v>EUR-EURIBOR-3M</v>
-      </c>
-      <c r="P8" s="20">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="P8" s="20" t="str">
         <f>_xll.og.Bean.property($L8,P$2)</f>
-        <v>0.26111111111111113</v>
-      </c>
-      <c r="Q8" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q8" s="24" t="str">
         <f>_xll.og.Bean.property($L8,Q$2)</f>
-        <v>2619250.9833476138</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="8" t="str">
         <f>_xll.og.RateCalculationSwapLeg.build(B10:B14,C10:C14)</f>
-        <v>RateCalculationSwapLeg@4</v>
+        <v>RateCalculationSwapLeg@1</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="8" t="str">
         <f>_xll.og.RateCalculationSwapLeg.build(G10:G14,H10:H14)</f>
-        <v>RateCalculationSwapLeg@3</v>
+        <v>RateCalculationSwapLeg@2</v>
       </c>
       <c r="L9" s="3" t="str">
-        <v>IborRateSensitivity@15</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M9" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L9,M$2))</f>
-        <v>EUR</v>
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
       </c>
       <c r="N9" s="20" t="str">
         <f>_xll.og.Bean.property($L9,N$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O9" s="23" t="str">
         <f>_xll.og.Bean.property($L9,O$2)</f>
-        <v>EUR-EURIBOR-3M</v>
-      </c>
-      <c r="P9" s="20">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="P9" s="20" t="str">
         <f>_xll.og.Bean.property($L9,P$2)</f>
-        <v>0.25277777777777777</v>
-      </c>
-      <c r="Q9" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q9" s="24" t="str">
         <f>_xll.og.Bean.property($L9,Q$2)</f>
-        <v>2537297.6014800463</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
@@ -2197,153 +2215,153 @@
         <v>20</v>
       </c>
       <c r="L10" s="3" t="str">
-        <v>IborRateSensitivity@16</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M10" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L10,M$2))</f>
-        <v>EUR</v>
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
       </c>
       <c r="N10" s="20" t="str">
         <f>_xll.og.Bean.property($L10,N$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O10" s="23" t="str">
         <f>_xll.og.Bean.property($L10,O$2)</f>
-        <v>EUR-EURIBOR-3M</v>
-      </c>
-      <c r="P10" s="20">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="P10" s="20" t="str">
         <f>_xll.og.Bean.property($L10,P$2)</f>
-        <v>0.25277777777777777</v>
-      </c>
-      <c r="Q10" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q10" s="24" t="str">
         <f>_xll.og.Bean.property($L10,Q$2)</f>
-        <v>2455273.4145536497</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>C16</f>
-        <v>PeriodicSchedule@3</v>
+        <v>PeriodicSchedule@1</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H11" s="1" t="str">
         <f>H16</f>
-        <v>PeriodicSchedule@4</v>
+        <v>PeriodicSchedule@2</v>
       </c>
       <c r="L11" s="3" t="str">
-        <v>ZeroRateSensitivity@9</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M11" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L11,M$2))</f>
-        <v>EUR</v>
-      </c>
-      <c r="N11" s="25">
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
+      </c>
+      <c r="N11" s="25" t="str">
         <f>_xll.og.Bean.property($L11,N$2)</f>
-        <v>0.25753424657534246</v>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O11" s="23" t="str">
         <f>_xll.og.Bean.property($L11,O$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="P11" s="20" t="str">
         <f>_xll.og.Bean.property($L11,P$2)</f>
-        <v/>
-      </c>
-      <c r="Q11" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q11" s="24" t="str">
         <f>_xll.og.Bean.property($L11,Q$2)</f>
-        <v>7933.4003224362186</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="str">
         <f>C22</f>
-        <v>PaymentSchedule@4</v>
+        <v>PaymentSchedule@2</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="1" t="str">
         <f>H22</f>
-        <v>PaymentSchedule@3</v>
+        <v>PaymentSchedule@1</v>
       </c>
       <c r="L12" s="3" t="str">
-        <v>ZeroRateSensitivity@10</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M12" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L12,M$2))</f>
-        <v>EUR</v>
-      </c>
-      <c r="N12" s="20">
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
+      </c>
+      <c r="N12" s="20" t="str">
         <f>_xll.og.Bean.property($L12,N$2)</f>
-        <v>0.50958904109589043</v>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O12" s="23" t="str">
         <f>_xll.og.Bean.property($L12,O$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="P12" s="20" t="str">
         <f>_xll.og.Bean.property($L12,P$2)</f>
-        <v/>
-      </c>
-      <c r="Q12" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q12" s="24" t="str">
         <f>_xll.og.Bean.property($L12,Q$2)</f>
-        <v>17071.727958181815</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>_xll.og.NotionalSchedule.build(B27:B28,C27:C28)</f>
-        <v>NotionalSchedule@4</v>
+        <v>NotionalSchedule@1</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="1" t="str">
         <f>H26</f>
-        <v>NotionalSchedule@6</v>
+        <v>NotionalSchedule@2</v>
       </c>
       <c r="L13" s="3" t="str">
-        <v>ZeroRateSensitivity@11</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M13" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L13,M$2))</f>
-        <v>EUR</v>
-      </c>
-      <c r="N13" s="20">
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
+      </c>
+      <c r="N13" s="20" t="str">
         <f>_xll.og.Bean.property($L13,N$2)</f>
-        <v>0.75890410958904109</v>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O13" s="23" t="str">
         <f>_xll.og.Bean.property($L13,O$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="P13" s="20" t="str">
         <f>_xll.og.Bean.property($L13,P$2)</f>
-        <v/>
-      </c>
-      <c r="Q13" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q13" s="24" t="str">
         <f>_xll.og.Bean.property($L13,Q$2)</f>
-        <v>25166.568677485251</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>_xll.og.FixedRateCalculation.of(D14,E14)</f>
-        <v>FixedRateCalculation@2</v>
+        <v>FixedRateCalculation@1</v>
       </c>
       <c r="D14" s="7">
         <v>0.01</v>
@@ -2356,100 +2374,100 @@
       </c>
       <c r="H14" s="1" t="str">
         <f>_xll.og.IborRateCalculation.of(I14)</f>
-        <v>IborRateCalculation@2</v>
+        <v>IborRateCalculation@1</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>71</v>
       </c>
       <c r="L14" s="3" t="str">
-        <v>ZeroRateSensitivity@12</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M14" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L14,M$2))</f>
-        <v>EUR</v>
-      </c>
-      <c r="N14" s="20">
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
+      </c>
+      <c r="N14" s="20" t="str">
         <f>_xll.og.Bean.property($L14,N$2)</f>
-        <v>1.0054794520547945</v>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O14" s="23" t="str">
         <f>_xll.og.Bean.property($L14,O$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="P14" s="20" t="str">
         <f>_xll.og.Bean.property($L14,P$2)</f>
-        <v/>
-      </c>
-      <c r="Q14" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q14" s="24" t="str">
         <f>_xll.og.Bean.property($L14,Q$2)</f>
-        <v>35787.13660480408</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
       <c r="L15" s="3" t="str">
-        <v>ZeroRateSensitivity@13</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M15" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L15,M$2))</f>
-        <v>EUR</v>
-      </c>
-      <c r="N15" s="20">
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
+      </c>
+      <c r="N15" s="20" t="str">
         <f>_xll.og.Bean.property($L15,N$2)</f>
-        <v>1.2575342465753425</v>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O15" s="23" t="str">
         <f>_xll.og.Bean.property($L15,O$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="P15" s="20" t="str">
         <f>_xll.og.Bean.property($L15,P$2)</f>
-        <v/>
-      </c>
-      <c r="Q15" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q15" s="24" t="str">
         <f>_xll.og.Bean.property($L15,Q$2)</f>
-        <v>43439.604779939771</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="8" t="str">
         <f>_xll.og.PeriodicSchedule.build(B17:B20,C17:C20)</f>
-        <v>PeriodicSchedule@3</v>
+        <v>PeriodicSchedule@1</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="8" t="str">
         <f>_xll.og.PeriodicSchedule.build(G17:G20,H17:H20)</f>
-        <v>PeriodicSchedule@4</v>
+        <v>PeriodicSchedule@2</v>
       </c>
       <c r="L16" s="3" t="str">
-        <v>ZeroRateSensitivity@14</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M16" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L16,M$2))</f>
-        <v>EUR</v>
-      </c>
-      <c r="N16" s="20">
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
+      </c>
+      <c r="N16" s="20" t="str">
         <f>_xll.og.Bean.property($L16,N$2)</f>
-        <v>1.515068493150685</v>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O16" s="23" t="str">
         <f>_xll.og.Bean.property($L16,O$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="P16" s="20" t="str">
         <f>_xll.og.Bean.property($L16,P$2)</f>
-        <v/>
-      </c>
-      <c r="Q16" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q16" s="24" t="str">
         <f>_xll.og.Bean.property($L16,Q$2)</f>
-        <v>54118.288769099832</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
@@ -2463,30 +2481,30 @@
         <v>42431</v>
       </c>
       <c r="L17" s="3" t="str">
-        <v>ZeroRateSensitivity@15</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M17" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L17,M$2))</f>
-        <v>EUR</v>
-      </c>
-      <c r="N17" s="20">
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
+      </c>
+      <c r="N17" s="20" t="str">
         <f>_xll.og.Bean.property($L17,N$2)</f>
-        <v>1.7643835616438357</v>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O17" s="23" t="str">
         <f>_xll.og.Bean.property($L17,O$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="P17" s="20" t="str">
         <f>_xll.og.Bean.property($L17,P$2)</f>
-        <v/>
-      </c>
-      <c r="Q17" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q17" s="24" t="str">
         <f>_xll.og.Bean.property($L17,Q$2)</f>
-        <v>61738.114744073675</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
@@ -2500,30 +2518,30 @@
         <v>43161</v>
       </c>
       <c r="L18" s="3" t="str">
-        <v>ZeroRateSensitivity@16</v>
+        <v>## Unable to convert argument to 'java.util.List'</v>
       </c>
       <c r="M18" s="20" t="str">
         <f>_xll.og.Currency.toString(_xll.og.Bean.property($L18,M$2))</f>
-        <v>EUR</v>
-      </c>
-      <c r="N18" s="20">
+        <v>## Argument 'currencyCode' with value '## Unable to convert argument to 'org.joda.beans.Bean'' must match pattern: [A-Z][A-Z][A-Z]</v>
+      </c>
+      <c r="N18" s="20" t="str">
         <f>_xll.og.Bean.property($L18,N$2)</f>
-        <v>2.0054794520547947</v>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="O18" s="23" t="str">
         <f>_xll.og.Bean.property($L18,O$2)</f>
-        <v/>
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
       </c>
       <c r="P18" s="20" t="str">
         <f>_xll.og.Bean.property($L18,P$2)</f>
-        <v/>
-      </c>
-      <c r="Q18" s="24">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+      <c r="Q18" s="24" t="str">
         <f>_xll.og.Bean.property($L18,Q$2)</f>
-        <v>68469.259415752371</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+        <v>## Unable to convert argument to 'org.joda.beans.Bean'</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
@@ -2537,13 +2555,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="1" t="str">
         <f>_xll.og.BusinessDayAdjustment.of(D20,E20)</f>
-        <v>BusinessDayAdjustment@3</v>
+        <v>BusinessDayAdjustment@1</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>7</v>
@@ -2556,7 +2574,7 @@
       </c>
       <c r="H20" s="1" t="str">
         <f>_xll.og.BusinessDayAdjustment.of(I20,J20)</f>
-        <v>BusinessDayAdjustment@4</v>
+        <v>BusinessDayAdjustment@2</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>7</v>
@@ -2565,25 +2583,25 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="8" t="str">
         <f>_xll.og.PaymentSchedule.build(B23:B24,C23:C24)</f>
-        <v>PaymentSchedule@4</v>
+        <v>PaymentSchedule@2</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H22" s="8" t="str">
         <f>_xll.og.PaymentSchedule.build(G23:G24,H23:H24)</f>
-        <v>PaymentSchedule@3</v>
+        <v>PaymentSchedule@1</v>
       </c>
       <c r="O22" s="22"/>
       <c r="Q22" s="6"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
@@ -2599,7 +2617,7 @@
       <c r="O23" s="22"/>
       <c r="Q23" s="6"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
         <v>9</v>
       </c>
@@ -2615,29 +2633,29 @@
       <c r="O24" s="22"/>
       <c r="Q24" s="6"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.35">
       <c r="O25" s="22"/>
       <c r="Q25" s="6"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B26" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="8" t="str">
         <f>_xll.og.NotionalSchedule.build(B27:B28,C27:C28)</f>
-        <v>NotionalSchedule@5</v>
+        <v>NotionalSchedule@3</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H26" s="8" t="str">
         <f>_xll.og.NotionalSchedule.build(G27:G28,H27:H28)</f>
-        <v>NotionalSchedule@6</v>
+        <v>NotionalSchedule@2</v>
       </c>
       <c r="O26" s="22"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
         <v>12</v>
       </c>
@@ -2653,7 +2671,7 @@
       <c r="O27" s="22"/>
       <c r="Q27" s="6"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
         <v>13</v>
       </c>
@@ -2670,12 +2688,12 @@
       <c r="O28" s="22"/>
       <c r="Q28" s="6"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.35">
       <c r="O29" s="22"/>
       <c r="Q29" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="Y6:Z29">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Y6:Z29">
     <sortCondition ref="Y6:Y29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>